<commit_message>
related tags for rappler
</commit_message>
<xml_diff>
--- a/rappler.xlsx
+++ b/rappler.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,22 +440,27 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>title</t>
+          <t>Title</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>Url</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>date_published</t>
+          <t>Publish Date</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>Content</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Related Topics</t>
         </is>
       </c>
     </row>
@@ -461,39 +470,977 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>PMA hazing leads to cadet’s 8-month hospital stay</t>
+          <t>YouTube removes nearly 11,000 propaganda channels linked to China, Russia, others</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://www.rappler.com/philippines/luzon/military-academy-hazing-cadet-hospital-2025/</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>2025-07-09T08:51:24+08:00</t>
-        </is>
+          <t>https://www.rappler.com/technology/youtube-propaganda-channel-removal-china-russia-second-quarter-2025/</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>45860.37956018518</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t xml:space="preserve">BAGUIO, Philippines – A 22-year-old cadet at the Philippine Military Academy (PMA) was allegedly subjected to weeks of physical abuse and psychological torment inside the campus in 2024, an ordeal that has now reached prosecutors after internal sanctions imposed by the military school.
-The victim stayed in a hospital for eight months as a result.
-The PMA confirmed on Monday, July 7, that the 4th class cadet was harmed in September 2024 while staying at Yap Hall, and said the case has been referred for possible criminal prosecution.
-“Nonetheless, we confirm that a thorough and impartial investigation was completed in accordance with our military justice system,” said Lieutenant Jesse Nestor Saludo, head of the PMA’s Public Affairs Office.
-The PMA said the cadets involved have been sanctioned under the Armed Forces and Cadet Corps regulations.
-Saludo said two were suspended while a squad leader was given the highest maximum demerit, confinement days, and punishment hours which he is continuously serving to date because it was his command responsibility.
-The police have brought the complaint to the local prosecutor’s office for possible charges under the Anti-Hazing Act of 2018.
-The incident followed the 2023 conviction of three PMA cadets for the 2019 hazing death of Darwin Dormitorio. The court sentenced them to reclusion perpetua, or up to 40 years in prison. Dormitorio’s death triggered public outcry and prompted institutional changes within the military school.
-The alleged 2024 abuse became public after the cadet filed a police blotter report on July 2 at Baguio City’s Police Station 4. 
-The complainant alleged that he was physically assaulted, forced to perform extreme physical exercises, and subjected to “animalistic tripping” by upperclassmen and classmates between September 2 and September 29, 2024.
-Police identified four cadets as suspects: one 1st class cadet, one from the 2nd class, and two 4th class cadets. 
-The victim alleged that the mistreatment began after an upperclassman ordered others to hit him under the pretense of training.
-The cadet also said he was frequently disturbed during sentinel duties and compelled to perform drills that resulted in physical collapse. On September 29, 2024, he was allegedly struck by a 1st class cadet and nearly lost consciousness.
-He was initially taken to the V. Luna Medical Center in Quezon City for treatment and later transferred to the PMA Station Hospital in Baguio, where he stayed until June 30, 2025. He remains on indefinite leave while awaiting a final discharge from the Armed Forces of the Philippines Medical Board.
-The PMA said it has not received a copy of the police report or formal civilian complaint but reiterated its position that it “does not condone maltreatment.” 
-It said reforms introduced since 2018 have improved training policies, supervision, and monitoring systems.
-The PMA urged the public to “continue placing their trust in the institution,” adding that it remains “unwavering in its commitment to providing quality education and training, and to developing principled and competent leaders who will honorably serve the Armed Forces of the Philippines and our nation.” – Rappler.com
-</t>
+          <t xml:space="preserve">SUMMARY This is AI generated summarization, which may have errors. For context, always refer to the full article. MANILA, Philippines – Google announced on Monday, July 21, it removed nearly 11,000 YouTube channels and other accounts in the second quarter of 2025 for “coordinated influence operation campaigns” on the service. In a bulletin post for Q2 2025 , it listed some 7,700 channels linked to Chinese propaganda. These included the termination of 1,545 YouTube channels in April, 3,592 YouTube channels in May, and 2,598 YouTube channels and the blockage of one domain from eligibility to appear on Google News surfaces and Discover in June. “The coordinated inauthentic network uploaded content in Chinese and English about China and US foreign affairs,” the post said. Meanwhile, more than 2,000 YouTube channels were removed in Q2 2025 for “coordinated influence operations linked to Russia.” These included content in multiple languages showing support for Russia and criticism for Ukraine, Poland, NATO, and the West. In May, the company also removed 20 YouTube channels, 4 Ads accounts, and 1 Blogger blog linked to Russian influence ops. In this case, the campaign was “linked to the Russian state-controlled media outlet RT and was sharing content in Spanish, English, Serbian, and Russian that was supportive of Russia and critical of Ukraine and the West.” Other removed influence campaigns were linked to Azerbaijan, Iran, Israel, Ghana, Romania, and Turkey and appeared to target political rivals or, as in Israel’s case here, to posit support for Israel and criticize Palestine. Google’s Threat Analysis Group removed more than 23,000 accounts in the first quarter of 2025, most notably more than 11,900 China-linked YouTube channels which discussed Chinese and US foreign affairs. – Rappler.com How does this make you feel? </t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>disinformation and misinformation,Fighting disinformation,Google,Misinformation on Youtube,Networked propaganda</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>[DECODED] Déjà vu: Parallels between US and Philippine propaganda</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>https://www.rappler.com/voices/newsletters/decoded-parallels-between-united-states-philippine-propaganda/</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>45714.41666666666</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SUMMARY This is AI generated summarization, which may have errors. For context, always refer to the full article. Have you been keeping up with all the issues surrounding USAID, or the US Agency for International Development? In my latest Decoded story , I wrote about the lies and conspiracy theories about the agency, and how these were spreading online following the Trump administration’s moves to shut it down. USAID is the US government’s arm that provides humanitarian assistance to several countries. But according to some social media posts, USAID is a criminal organization, a radical-left psy-op, and a vehicle that backs liberal or progressive groups that promote American propaganda. Sounds familiar? We know that all too well. In the Philippines, independent media outlets have long been attacked for receiving funding from US-based organizations, including USAID and the National Endowment for Democracy (NED). These outlets are accused of their supposed pro-US or Western bias, and of supposedly serving as fronts for the US Central Intelligence Agency (CIA). This isn’t the first time that American propaganda and disinformation have penetrated Philippine online spaces. Last year, I wrote about how Filipinos echoed American lies — from both sides of the political spectrum — about the assassination attempt on then-presidential candidate Donald Trump. After all, it is true that the Philippines is America’s guinea pig when it comes to social media propaganda and information operations. That’s because over 7 in 10 people in the Philippines are on social media, and these platforms are barely regulated in the country. Philippine and US politics also have many similarities. As Cambridge Analytica whistleblower Christopher Wylie put it , we had “a president who was Trump before Trump was Trump.” Concepts surrounding disinformation, propaganda, and fake news turned mainstream around 2016, following the presidential victories of Rodrigo Duterte and Donald Trump. Duterte “ institutionalized ” disinformation with sock puppet accounts and fake networks , while the first Trump victory was preceded by Russian information operations and outrageous conspiracy theories . In this 2019 Rappler exclusive, Wylie said the Philippines was the company’s “ petri dish ”  for testing their strategies before implementing them in Western countries. In the infamous Cambridge Analytica scandal, the Philippines ranked second to the US in terms of the number of Facebook users whose data was compromised. Duterte and Trump are also both sharp-tongued populists who frequently hurled attacks towards critics and sowed distrust in democratic institutions. Duterte falsely claimed in 2017 that the CIA funds Rappler, and now Trump is baselessly claiming that USAID is run by “radical left lunatics.” There’s no denying that America’s been a strong influence on the Philippines, for better or for worse. These patterns aren’t limited to the Philippines and the US. Rappler CEO Maria Ressa previously talked about how 2024 was a “ super-election year ” with 74 national elections globally, which saw the loss of many of the world’s incumbents and the proliferation of more insidious voter manipulation on social media. Next week, our lead forensics researcher Pauline Macaraeg will be publishing a story on the rise of right-wing populist narratives in Canada as the country prepares for the federal election slated for October 20 this year. Any other parallels you’ve noticed? Let us know by sending us an email at hello@thenerve.co. – Rappler.com [DECODED] What the Pepsi Paloma movie could mean for Tito Sotto’s Senate bid While the film’s trailer doesn’t name Tito Sotto, data from The Nerve shows that 30% of recent online discussions about him revolve around Paloma . [DECODED] The lies, attacks on USAID spreading in the Philippines Conspiracy theories claim USAID backs media outlets and organizations that promote US interests and liberal agendas . [DECODED] Understanding voters’ behavior for the 2025 senatorial elections A survey by The Nerve classifies 2,700 respondents who are Rappler readers into four groups: practical working class, economy-conscious professionals, young progressives, and law-and-order rural supporters . The Nerve is a data forensics company that enables changemakers to navigate real-world trends and issues through narrative and network investigations. Taking the best of human and machine, we enable partners to unlock powerful insights that shape informed decisions. Composed of a team of data scientists, strategists, award-winning storytellers, and designers, the company is on a mission to deliver data with real-world impact. Visit and bookmark Rappler’s 2025 Philippine elections site for the latest news, explainers, analyses, multimedia content, and data on the senatorial, party list, and local contests. How does this make you feel? </t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Decoded,Disinformation,Donald Trump,Fighting disinformation,foreign aid,Networked propaganda,Rodrigo Duterte,US foreign aid</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>[DECODED] Do politicians need facts when they have propaganda armies?</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>https://www.rappler.com/philippines/elections/decoded-politicians-need-facts-propaganda-armies/</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>45686.41666666666</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SUMMARY This is AI generated summarization, which may have errors. For context, always refer to the full article. What comes to mind when you think of disinformation and propaganda? Chances are, you’ll start thinking of power-hungry politicians spreading lies about their legacy or bloggers and influencers incessantly attacking opposition leaders and other figures critical of the administration. Maybe you remember the 2022 presidential elections, which saw the son of a dictator win the support of millions of Filipinos and eventually the presidency. As a digital forensics researcher who wrote several stories about election-related propaganda in the first few months of 2022, that’s what I remember the most about that period. Now we’re back in an election landscape as we prepare for the upcoming 2025 midterm polls and brace for more disinformation and propaganda-fueled campaigns. Reinnard Balonzo, one of Rappler’s Aries Rufo Journalism fellows for 2024, wrote a two-part story about the media and information landscape in the Bicol region. His stories showed that political disinformation is a multifaceted problem. First, he pointed out the pitfalls of the region’s media landscape — where local media paints politicians as heroes, where there aren’t enough independent media organizations, and where community journalists are under attack. He also talked about how political movements exploit poor Bicolanos . Welfare programs in the region are used for politicians’ premature campaigns and volunteer-led youth organizations openly endorse certain leaders. Many Bicolanos also get their information from social media platforms rife with disinformation because they can’t afford anything else. I’m not a fan of the “bobotante” narrative that pins the blame on poor voters; the situation’s always more complicated than that. These Bicolanos often have little choice but to become victims of political machineries. And we all know how political machineries endorsing national candidates can be vicious. In my latest Decoded story , I explored how the Duterte supporter base on social media came to the defense of Vice President Sara after everything she went through in 2024 . This included an investigation into her alleged misuse of confidential funds , three  impeachment  complaints , and a drop in approval ratings . But to her most loyal supporters, the Vice President is an indestructible leader who’s being unfairly persecuted. What made writing this story so interesting was that all of this unfolded in the wake of Duterte’s public breakup with President Ferdinand Marcos Jr. The Dutertes and Marcoses are both notorious for their disinformation and propaganda networks on social media, so I wanted to see who was winning the battle on Facebook. (Hint: It’s not the President.) Sure, Duterte has three more years to go until her vice presidential term ends, but she could also be laying the groundwork for the next presidential election as early as now. And if there’s anything we at The Nerve learned about studying disinformation on social media, it’s that we need to keep an eye out before it’s too late. Have you seen any political disinformation or propaganda narratives we should be looking into? Let us know by sending us an email at hello@thenerve.co. – Rappler.com [DECODED] Duterte social media army very much alive, roars to defend embattled Sara Duterte On Facebook, pro-Duterte accounts portray Vice President Sara Duterte as a larger-than-life, indestructible leader . [DECODED] Goodbye fact-checkers? Hello to more lies! By dismissing fact-checking as ‘biased,’ Zuckerberg undermines the work of journalists . [DECODED] What songs and artists did Filipinos listen to in 2024? Spotify chart data shows that Filipino hip-hop and P-pop acts were among the most-streamed for listeners across the country . The Nerve is a data forensics company that enables changemakers to navigate real-world trends and issues through narrative and network investigations. Taking the best of human and machine, we enable partners to unlock powerful insights that shape informed decisions. Composed of a team of data scientists, strategists, award-winning storytellers, and designers, the company is on a mission to deliver data with real-world impact. How does this make you feel? </t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2025 Philippine elections,Bicol,Decoded,disinformation and misinformation,Fighting disinformation,Philippine politics,Sara Duterte,social media,social media influencers</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>[DECODED] Who’s afraid of Gen Z?</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>https://www.rappler.com/voices/newsletters/decoded-who-is-afraid-gen-z/</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>45644.41666666666</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SUMMARY This is AI generated summarization, which may have errors. For context, always refer to the full article. Let’s face it: Gen Z might just be the most misunderstood generation in recent history. Hi! I’m Gaby Baizas, a 27-year-old digital forensics researcher for Rappler and The Nerve — and the only Gen Z in our digital forensics team. I’m here to share what we’ve uncovered about my generation, one story at a time. Over the past year, we’ve explored how Gen Zs think about some of the most pressing issues today. If you’re Gen Z, I hope these stories resonate with you. If you’re from another generation, I hope they give you a deeper understanding of what makes us tick. Around this time last year, I wrote an in-depth data story that looked into the socioeconomic factors that impacted Gen Z’s attitudes on work and money. I’ve always heard older generations share their misgivings about our work ethics and attitudes. But I understood that these shifts in workplace behaviors didn’t just come out of nowhere; they were brought about by a dwindling economy and fears that we might not be able to afford basic needs or emergencies. When we officially launched Decoded in July, our lead forensics researcher Pauline Macaraeg wrote about how these financial fears bled into young couples’ decisions to not have children. The DINK (dual income, no kids) phenomenon shows that Gen Z and even millennial couples have a deep understanding of the financial and personal commitments that come with starting a family. Brands could learn from Gen Z’s beliefs and preferences, too. We’ve also written about how sustainability matters to Gen Z TikTok users in Southeast Asia, among the most vulnerable regions to climate change . TikTok users prefer smaller brands and influencers when it comes to eco-friendly products and practices, and are often skeptical of larger companies that might engage in greenwashing practices. But one of the most significant findings we’ve written about is how Gen Z’s high social media use can make us susceptible to online manipulation. Sure, Gen Zs like me spend a lot of time on social media and are more familiar with newer technologies, but that doesn’t mean we’re immune to propaganda online. For instance, Rappler digital communications specialist Laurice Angeles wrote about how she first learned about ADHD through social media , and how this prompted her to seek professional help. While platforms like TikTok could raise awareness on certain health conditions, Gen Z users who substitute medical appointments with social media advice could put themselves and their health at risk. After all, social media platforms are rife with unverified claims. If you’ve been keeping up with The Nerve’s work, you might be familiar with our forensics research on disinformation. In our last newsletter, Don Kevin Hapal, who led the project, discussed our study on the US information ecosystem. Ahead of last November’s election, we found a growing generational divide: while older voters stuck to more traditional news sources, younger voters were relying heavily on social media. This means young Americans voters are exposed to hyperpartisan manipulation and disinformation online, which might also be why they also turned out to be the most divided on key election issues, and who they voted for in the elections. (You can download the full report here .) No matter how you feel about Gen Z, there’s no denying that this generation really found its voice this year. We’ve dominated discourse on global conflicts, raised awareness on environmental issues, and led cultural revolutions that have become too big and significant for other generations to ignore. What do you think about Gen Z? If you’re interested in Nerve and have ideas on how we can work together, feel free to email us at hello@thenerve.co. For more information, you can also visit our website . – Rappler.com The Nerve is a data forensics company that enables changemakers to navigate real-world trends and issues through narrative and network investigations. Taking the best of human and machine, we enable partners to unlock powerful insights that shape informed decisions. Composed of a team of data scientists, strategists, award-winning storytellers, and designers, the company is on a mission to deliver data with real-world impact. How does this make you feel? </t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>disinformation and misinformation,Networked propaganda,Philippine economy,social media,social media platforms</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Pro-China propaganda pivots, targets civil society as tensions mount</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>https://www.rappler.com/newsbreak/investigative/pro-china-propaganda-pivots-targets-philippines-civil-society-tensions-mount/</t>
+        </is>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>45532.48958333334</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SUMMARY This is AI generated summarization, which may have errors. For context, always refer to the full article. This story was made in collaboration with data forensics company The Nerve . In the ongoing saga that sees the Philippines on the receiving end of Chinese harassment, China-linked propaganda pushes the narrative that the country is caught in a proxy war initiated by the United States. The official Facebook accounts of China state-affiliated entities and media are among the sources of these propaganda narratives online, as found in a scan of posts from June 2022 to July 2024, under the administration of President Ferdinand Marcos Jr. The scan was conducted by Rappler and data forensics company The Nerve. These narratives include blaming the US for China’s rift with other countries, targeting the so-called “Western media.” Such propaganda highlights China’s supposed sovereignty over countries they claim as their own and emphasizes the importance of a regional alliance among Asian countries against the West. They also target civil society movements that attempt to stand up to Chinese harassment in the West Philippine Sea. With the continuing Chinese harassment of Filipino vessels and the Philippine Coast Guard (PCG), however, the pro-China narratives are trumped by the overwhelming anti-China sentiment from individuals trooping to social media to voice their support. Akbayan Party president Rafaela David, who is also a co-convenor of civilian-led advocacy Atin Ito, said that the China propaganda campaign “is designed to belittle the courage of the ordinary Filipinos and the efforts of legitimate civil society organizations.” The public sentiment also lines up with the Philippine government’s more decisive actions against China’s harassment and other acts of intimidation. This stronger stance of government under President Marcos is different from the often inconsistent, if not outrightly dismissive, Duterte administration. The increasing tension between the Philippines and China has inspired ordinary citizens to voice out their disapproval of China’s moves. But a coalition of civil society organizations took this a notch higher by actually sailing out to sea to assert ordinary Filipinos’ rights. The Atin Ito coalition has done two civilian missions so far. The civilian-led convoy first set sail in December 2023 to Ayungin Shoal to deliver supplies to military and Philippine Coast Guard (PCG) outposts, but eventually had to turn back due to the “ constant shadowing ” of China vessels. In May 2024, the convoy went on another civilian supply mission to deliver food and fuel to Filipino fishermen “to show solidarity and support to the community who are most affected by what China is doing in our own waters.” David said that the mission sought to “normalize and regularize civilian access” in the West Philippine Sea to counter China’s militarization. “Let it be made clear, Filipinos have agency [and] we do not need other foreign powers to compel us to do what is the inherent responsibility of every Filipino citizen [which is] to defend our country and protect our own rights,” David told Rappler. But Facebook pages found to have links to China paint another story. For these propaganda arms, the Atin Ito coalition and its missions are pawns supposedly deployed by the US and the Philippine governments. State-controlled media China Daily on May 15, posted a Facebook video baselessly claiming that the coalition “is actually secretly funded by the Philippines and the US governments,” as it questioned how a small civic group was able to mobilize resources for these missions. The one-minute video linked the Atin Ito efforts to a so-called Project Myoushu, an initiative that started in 2022 at the Gordian Knot Center for National Security Innovation at Stanford University. The Gordian Knot Center’s website states that the project is sponsored by the US Office of Naval Research. In a separate video posted a month later on June 15, China Daily presented more details about the alleged project, saying it is “funded by the Philippines and the US governments to bolster the Philippines’ position in the South China Sea.” According to Ray Powell, analyst and Project Myoushu lead, the project wanted to take a “fresh look” at the South China Sea issue and saw that most of the country’s “maritime aggressions were enabled by the fact that most of them took place out of the public view.” The China Daily video said that the project “portrays China as an aggressor, aiming to suppress narratives that challenge the Western discourse.” These baseless claims have also been shared in various online communities via coordinated, inauthentic behavior. Rappler found that a handful of Facebook accounts had coordinately shared popular posts from China-affiliated pages, amplifying propaganda surrounding the Atin Ito coalition. Such posts were being seeded into three significant communities — groups supporting China or the BRICS countries (led by Brazil, Russia, India, China, and South Africa), Philippine political groups, and buy-and-sell groups. The pro-China/BRICS and Philippine political Facebook groups explicitly include names of politicians, parties, and other institutions supportive of China. Some Philippine political groups mention President Marcos and his party, Partido Federal ng Pilipinas, as these groups were named in the lead up to the 2022 elections, where Marcos and Sara Duterte forged ties. A previous Rappler investigation found that it did not take long for the Marcos and Duterte networks to crack after the President took a more pro-US foreign policy approach. However, pro-China propaganda still found its way to a number of buy-and-sell groups, which are extremely active and likely not closely moderated, despite some groups having a “no-spam” rule. The smallest of these buy-and-sell groups has over 19,700 members, while the largest has over 486,500 members. These groups can have hundreds or thousands of new posts every day, making it easier for unrelated posts to slip through the cracks. The scan by Rappler and The Nerve showed that CRI Filipino Service, tagged by Facebook as “China state-controlled media,” was the first China-linked page that mentioned Project Myoushu. It posted on December 19, 2023 an announcement about a forum that aimed to tackle how “US Project Myoushu-PBBM rapes RP.” The speakers are known to have links with China. Three of the named speakers “were among the network of supposed experts who would push for Beijing’s narratives” and “would be consistently cited and interviewed in Chinese state media,” according to the book, Unrequited Love: Duterte’s China Embrace by journalists Marites Vitug and Camille Elemia. Previous Rappler findings showed that pro-China propaganda in the Philippines often came from bloggers and websites that claimed academic expertise and legitimacy. CRI Filipino Service went on to post about Project Myoushu four more times — another one in December 2023, once in January 2024, and twice in May 2024. In a post published on May 15, 2024, CRI Filipino claimed that Project Myoushu uses social media to spread false information about normal Chinese vessel activities in the South China Sea. The Chinese embassy in Manila also explicitly mentioned Project Myoushu in a post on May 16, 2024. It posted a link to a Global Times opinion piece that tagged the Atin Ito coalition as “far from being genuinely civilian,” claiming that it was “another act in the US’ Project Myoushu.” China-linked or affiliated pages are not the only ones posting allegations against the Atin Ito coalition and the bigger Project Myoushu conspiracy. A search on Facebook showed that the narrative related to Project Myoushu has been carried by individual bloggers and pages that have links to, or show apparent support for, Rodrigo Duterte, his allies, or the previous administration as a whole. One of the individuals who consistently posts about the project and its link to the Atin Ito coalition is a writer named Elmer Jugalbot. On May 15, Chinese state-run news site CGTN’s Facebook page published a video interview with Jugalbot , where he claimed that the civilian mission was funded by the US through Project Myoushu. Jugalbot, who identifies himself as a “political commentator,” has been cited in articles published by China-run or China-linked media, including CRI Filipino Service. He has also been featured in several videos published by SMNI News, owned by fugitive and Duterte ally Apollo Quiboloy. Before this, a certain Jugalbot was referred to by a 2018 news report as a “ businessman ”. Atin Ito’s David denied that the civilian group has any links with Project Myoushu, claiming that these allegations from China-linked pages “are as fictitious as their 9-dash line.” “Such absurd lies only show that they are threatened by ordinary Filipinos who dared to come together and hold accountable a superpower like China,” she told Rappler. Project Myoushu’s Powell also said “there is no connection whatsoever” between the project and the Atin Ito coalition. He said that the online narrative “suggests an orchestrated messaging campaign” that is aligned with China. Atin Ito’s David said that China’s narrative comes as no surprise, given how the civilian movement in the Philippines has since increased. “China’s lies seek to divide us, and sow doubt among civilian groups who found the collective courage to stand up against a bully like China,” she said. “By seeking to discredit legitimate civilian dissent to their illegal activities, they aim to dampen Filipinos’ resolve to stand up for what is rightfully ours.” The claims against civilian missions carried out by the Atin Ito coalition are just part of a bigger narrative deployed on social media as tensions escalate. For many Filipino netizens, it’s a no-brainer to support the cause and express patriotism through social media comments on Philippine-based media organizations’ news reports about the tensions. But Rappler and The Nerve also found a handful of social media comments that framed the issue as if the Philippines was starting a war that it is not ready for. Several Facebook users alluded to China as a global superpower that had all the resources, while the Philippines had nothing to show. There is also the narrative that alleges that the Philippines is just caught in a proxy war initiated by the US. Information released by authorities indicating incidents committed by Chinese vessels or the CCG against Filipino vessels were tagged as “Western war-mongering propaganda” and “another drama directed by the US.” They also accuse the US of “not supporting the Philippines but…escalating the tension.” Patterns of inauthentic behavior were also observed in the accounts posting this content. One account was found spamming rapid, continuous, and repetitive comments showing screenshots of anti-US content to different posts — a technique previously identified as part of the Russian “Firehose of Falsehood” Propaganda Model . While China-linked pages are now increasingly extending their narrative to also focus on civic society, and even warmongering, ordinary Filipinos online are hitting back by also consistently asserting Philippine rights and condemning Chinese harassment. This is evident on TikTok, where videos expressing support for Atin Ito and condemning Chinese aggression are among the most talked about and most liked. The Nerve analyzed 568 TikTok videos containing hashtags related to the West Philippine Sea by processing their audio, converting them into text, and applying natural language processing for narrative analysis. ( EDITOR’S NOTE: An earlier version of this story said 359 TikTok videos were analyzed. This has been corrected. ) Among the videos that were played the most were reports on the successful ventures of the Atin Ito movement and the favorable reaction of the international community toward the Philippines. Memes were also among the most shared videos, including posts making fun of Vice President Sara Duterte for her “no comment” quip when asked about the ongoing bullying by China. Political analyst and professor of political science Arjan Aguirre said that perhaps one of the reasons why pro-China propaganda carried by official outlets does not sway Filipinos — or the general public — is because “they are devoid of effective communicative devices.” He said that the messages are “usually poorly constructed” or there is an “effort to limit the scope of the discussion to topics that are innocuous to them.” “In fact in the subconscious of many of us, we already know that movements need resources and if it is true that the US is funding this movement, people would just feel good about the info that someone is helping us against China,” he said. “This is another layer, a pragmatic sense, that I’m getting or sensing about the issue.” Can we expect China to take its propaganda efforts up a notch? – Rappler.com This investigation used Nerve’s suite of forensic solutions including video and network analysis. If you’re interested in working with the Nerve, send an email to hello@thenerve.co. The Nerve is a data forensics company that enables changemakers to navigate real-world trends and issues through narrative &amp; network investigations. Taking the best of human and machine, we enable partners to unlock powerful insights that shape informed decisions. Composed of a team of data scientists, strategists, award-winning storytellers and designers, the company is on a mission to deliver data with real-world impact. How does this make you feel? </t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Decoded,Networked propaganda,social media,social media platforms,South China Sea</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Meta says it removed China-based propaganda operation targeting US midterms</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>https://www.rappler.com/technology/social-media/meta-removes-china-based-propaganda-operation-targeting-united-states-midterms/</t>
+        </is>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>44832.03802083333</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SUMMARY This is AI generated summarization, which may have errors. For context, always refer to the full article. META. The logo of Meta Platforms is seen in Davos, Switzerland, on May 22, 2022. Arnd Wiegmann/Reuters Meta Platforms said on Tuesday, September 27, it disrupted the first known China-based influence operation focused on targeting users in the United States with political content ahead of the midterm elections in November. The network maintained fake accounts across Meta’s social media platforms Facebook and Instagram, as well as competitor service Twitter, but was small and did not attract much of a following, Meta said in a report summarizing its findings. Still, the report noted, the discovery was significant because it suggested a shift toward more direct interference in US domestic politics compared with previous known Chinese propaganda efforts. “The Chinese operations we’ve taken down before talked primarily about America to the world, primarily in South Asia, not to Americans about themselves,” Meta global threat intelligence lead Ben Nimmo told a press briefing. “Essentially the message was ‘America bad, China good,'” he said of those operations, while the new operation pushed messages aimed at Americans on both sides of divisive issues like abortion and gun rights. Another Meta executive at the briefing said the company did not have enough evidence to say who in China was behind the activity. Asked about Meta’s findings at a news conference, U.S. Attorney General Merrick Garland said his office was “very concerned” about intelligence reports of election interference by foreign governments “starting back some time ago and continuing all the way into the present.” A Twitter spokesperson said the company was aware of the information in Meta’s report and also took down the accounts. According to Meta’s report, the Chinese fake accounts posed as liberal and conservative Americans in different states. They posted political memes and lurked in the comments of public figures’ posts since November 2021. A sample screenshot showed one account commenting on a Facebook post by Republican Senator Marco Rubio, asking him to stop gun violence and using the hashtag #RubioChildrenKiller. The same network also set up fake accounts that posed as people in the Czech Republic criticizing the Czech government over its approach to China, according to the report. Meta also said it had intercepted the largest and most complex Russian-based operation since the war in Ukraine began, describing it as a sprawling network of more than 60 websites impersonating legitimate news organizations, along with about 4,000 social media accounts and petitions on sites like US-based campaign group Avaaz. That operation primarily targeted users in Germany, as well as France, Italy, Ukraine and the United Kingdom, and spent more than $100,000 on ads promoting pro-Russian messages. On a few occasions, Russian embassies in Europe and Asia amplified the content. – Rappler.com How does this make you feel? </t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Networked propaganda</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Tracking the Marcos disinformation and propaganda machinery</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>https://www.rappler.com/newsbreak/iq/stories-tracking-marcos-disinformation-propaganda-machinery/</t>
+        </is>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>44665.125</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SUMMARY This is AI generated summarization, which may have errors. For context, always refer to the full article. MANILA, Philippines – As the 2022 polls inch closer, the online landscape becomes more difficult to navigate due to the deluge of disinformation that has favored the frontrunner of the presidential race – the dictator’s son, Ferdinand “Bongbong” Marcos Jr. Marcos has maintained a wide lead over his opponents even though he took longer to ramp up ad spending , is perpetually absent during presidential debates organized by major media organizations and the poll body, and has faced plenty of controversies involving his candidacy , his educational background , and his estate tax liability , among others. How does he sustain and gain support online? His camp and his supporters employ tactics that involve spreading lies and utilizing networks that platforms are too slow to stop. It is a years-long effort that will come to a head on May 9, when Filipinos will cast their votes. Here are Rappler investigations and reports on the many ways propaganda and disinformation related to the Marcoses thrive on social media, how platforms either respond or allow it to happen, and how the Marcos family benefits from the lies and manipulation. – Rappler.com How does this make you feel? </t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2022 PH presidential race,Disinformation,Ferdinand E. Marcos,Ferdinand Marcos Jr.,Marcos family,Networked propaganda</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Quiboloy’s SMNI fuels disinformation, online attacks on gov’t critics</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>https://www.rappler.com/technology/social-media/apollo-quiboloy-sonshine-media-network-disinformation-attacks-government-critics/</t>
+        </is>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>44598.33333333334</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SUMMARY This is AI generated summarization, which may have errors. For context, always refer to the full article. This story was made in collaboration with data consultancy TheNerve . MANILA, Philippines – Almost two years after ABS-CBN went off-air , the National Telecommunications Commission (NTC) distributed to other entities the frequencies previously assigned to the media giant. Among those awarded the frequency bands is Sonshine Media Network International (SMNI) , owned by President Rodrigo Duterte’s embattled friend, preacher Apollo Quiboloy. Quiboloy has long been mired in scandals, having been accused of land grabbing and indicted for sex trafficking , landing him on the most wanted list of the United States Federal Bureau of Investigation. A Rappler investigative series also found that ex-members of his church, the Kingdom of Jesus Christ (KOJC), were deep in debt due to his financial demands and had suffered emotional and psychological abuse. Read Rappler’s investigative series on Quiboloy here: Now, his church’s broadcasting arm is receiving government favor in the form of airwaves despite its failure to abide by journalistic standards. The Facebook page of its news and public affairs network, SMNI News, is at the core of the network of accounts, pages, and websites that red-tag government critics and attack the media. It also has a history of sharing misleading information and lending its platforms to hyper-partisan figures. On several occasions, SMNI News has been used as a platform to attack journalists and red-tag government critics. When ABS-CBN was denied a franchise after repeated threats from President Duterte, SMNI News published a report on Quiboloy urging the network’s supporters not to blame the government, but the network’s management for “not [doing] their job.” On SMNI’s Usaping Bayan program, host Mike Abe also told ABS-CBN’s supporters that, no matter how much they rally, Congress would not be able to easily renew ABS-CBN’s franchise. SMNI News has also allotted considerable airtime to congressmen Mike Defensor and Rodante Marcoleta , two key legislators who blocked ABS-CBN’s franchise renewal. They host SMNI’s Point of Order program, which they used to revisit ABS-CBN’s alleged violations a year after the license denial. Despite Defensor and Marcoleta’s claims, other government officials have cleared ABS-CBN of alleged violations, saying the network had regularly complied with tax requirements, labor standards, and franchise terms. Quiboloy himself compared ABS-CBN to the Communist Party of the Philippines-New People’s Army (CPP-NPA) due to their alleged “bias.” This came after supporters from a Marcos-Duterte motorcade crowded ABS-CBN vehicles, visibly annoying crew members. When Rappler CEO Maria Ressa received her Nobel Peace Prize in Norway, she talked about the persecution endured by journalists from Rappler and other newsrooms worldwide. In another Usaping Bayan broadcast, Abe had called Ressa a liar, slammed her for being dramatic in front of the international community, and questioned her Filipino citizenship. Ressa is a dual citizen who holds both Filipino and US citizenship. Attacks against journalists are repeated by SMNI’s readers. Duterte supporters often share SMNI’s content and slam mainstream media outlets for supposedly being “biased” against the administration, and for supposedly not reporting on certain government accomplishments. SMNI News is in the middle of the network of pages, accounts, and websites that have shared and created posts that attacked the media. Rappler scanned public posts from January 1, 2016, to October 31, 2021, to study posts with mentions of attack words we have collected over years of monitoring online harassment against the press. These words included “presstitute (a portmanteau of press and prostitute),” “bayaran (paid hacks),” and “bias,” among others. The maps above show the network of pages, accounts, and websites that harassed journalists online from 2020 to 2021. The blue circles represent the sources and sharers of the posts that contained attack keywords. The bigger the circle, the more it was shared by other actors in the network. The dark blue circles are the sources, or those who produced content, while the light blue circles represent those who shared content from the sources. SMNI News’ influence in the network became bigger starting in 2020. This was also the year that its Facebook page’s followers and page likes started to ramp up, based on data from CrowdTangle. Its Facebook page now has over 400,000 likes and more than 900,000 followers, as of February 3, 2022. An earlier Rappler investigation also found that SMNI News was among the top content sources of red-tagging networks. Clips of SMNI News’ reports about the CPP-NPA were shared by a network of pages and accounts that justified violence by branding activists and government critics as “terrorists.” SMNI News’ reports often only featured voices from government officials and allies. These reports were then shared by pages and accounts that captioned their posts with statements that blamed the media and institutions, like the Commission on Human Rights, for the supposed communist threat in the country – which they exaggerate. These posts also often contained unverified claims and presented them as facts, such as the accusation that actress Angel Locsin’s sister was a member of the NPA , and that the mainstream media had supposedly been “infiltrated” by communists . Leftist groups, particularly those that belonged to the Makabayan bloc , were also a top target of these accounts. The posts that shared SMNI News’ posts antagonized leftist groups and justified the attacks made on its members, drowning out the real stories of activists being harassed and killed . SMNI News pushed this narrative offline too. During the filing of candidacies for the 2022 polls, SMNI’s staff repeatedly asked members of the Makabayan bloc about their alleged communist ties – a line of questioning critics had flagged as dangerous and tantamount to red-tagging. SMNI News has also reported misleading and outright false claims, which have been fact-checked by third-party fact-checkers. These included a quote card of Vice President and presidential contender Leni Robredo which lacked context, as well as a report that claimed dictator’s son Ferdinand “Bongbong” Marcos Jr. “passed” his bachelor’s degree in social studies at the University of Oxford . The network has also lent their platforms to politicians and personalities who often make false claims – in effect, SMNI does not directly make the claims, the interviewees do. In an Usaping Bayan broadcast in 2020, Senator Imee Marcos falsely claimed that the equipment of the Bataan Nuclear Power Plant was gone – a claim Rappler later fact-checked . SMNI News also gives commentary programs to public officials and bloggers , including RJ Nieto of Thinking Pinoy and Sass Sasot, who use their platforms to spread government propaganda. SMNI News has distanced itself from the mainstream media. Though it usually publishes content in favor of the Duterte administration, it describes itself as “a true alternative network that broadcasts the uncompromising message of truth giving emphasis to responsible journalism and broadcasting; driven with the purpose to satisfy man’s spiritual need leading to transformation and excellent service,” as stated in its Facebook page. SMNI is also a member of ​​Kapisanan ng mga Brodkaster ng Pilipinas (KBP), whose broadcast code provides networks and media outfits ethical guidelines and standards for both news and commentary programs. The KBP encourages the public to submit complaints via their website whenever member stations violate guidelines listed in the code. Those who violate the code are subject to penalties and other sanctions. Individuals who violate the code can receive temporary suspensions and can have their accreditation revoked, while stations can be censured and given temporary suspensions of member privileges. However, SMNI News continues to broadcast freely, and its hosts continue to amplify lies and propaganda even on social media. SMNI’s strategy of featuring pro-administration figures and propaganda should not come as a surprise, as Quiboloy is a longtime friend and spiritual adviser of President Duterte. The network’s roots trace back to early radio and television programs by the media ministry of Quiboloy’s KOJC. Legally known as the Swara Sug Media Corporation, SMNI was first granted a franchise when bills lapsed into law in 1995. In May 2016, the network launched SMNI News, and in 2019 Duterte signed their franchise extension , allowing them to operate for another 25 years, or until 2044. Quiboloy actively campaigned for Duterte and lent him a private plane during the 2016 national election. The pastor even predicted a landslide victory for Duterte, saying he was the leader the Philippines needed to “slay corruption, drug addiction, and poverty.” Duterte also admitted that he received other lavish gifts from Quiboloy, including properties and cars, but said that these donations were made “in the name of God.” Most recently, Quiboloy officially endorsed the tandem of dictator’s son Ferdinand “Bongbong” Marcos Jr. and presidential daughter Sara Duterte for the upcoming 2022 election. He predicted that Marcos and Duterte, the current survey frontrunners, would also enjoy a landslide win. Both Quiboloy and Duterte enjoy exaggerated, cultish devotion from their followers, to the extent that their wrongdoings are tolerated or go unchecked. Before Rodrigo Duterte was sworn into office, Quiboloy had said he would not use their longtime friendship to meddle with issues of “national interest.” Duterte had said the same about his friendships, saying “My loyalty to you as a friend ends where my loyalty to my country begins.” Over five years later, the NTC, the same executive agency that shut down media giant ABS-CBN, granted Quiboloy’s SMNI a wider reach with highly-coveted frequencies – never mind if its network incites hate and spreads propaganda. – with reports from Gemma B. Mendoza, Don Kevin Hapal, Dylan Salcedo/Rappler.com This study was made in collaboration with TheNerve , a Manila-based consultancy that specializes in analyzing data to bring forth powerful insights and narratives. Believing that data can deliver real-world impact, the company enables its partners across a wide range of industries to cut through the clutter and extract value and meaning from various datasets. The insights guide partners’ business decisions and help them engage with their communities better. Composed of a team of data scientists, business strategists, award-winning storytellers, and designers, the company is on a mission to transform data science into data relevance. How does this make you feel? </t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>#FactsFirstPH research,digital forensics,Fighting disinformation,media industry</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Study finds signs of ‘networked political manipulation’ on social media</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>https://www.rappler.com/philippines/elections/study-finds-sign-networked-political-manipulation-social-media-digital-public-pulse-project/</t>
+        </is>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>44594.4956712963</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SUMMARY This is AI generated summarization, which may have errors. For context, always refer to the full article. Nico Villarete/Rappler MANILA, Philippines – The Digital Public Pulse (DPP) project’s landscape analysis of YouTube, Facebook, and Twitter found five indicators of “networked political manipulation” in relation to the 2022 elections. The researchers at the Philippine Media Monitoring Laboratory announced their findings on Wednesday, February 2. This is the fourth report of the first phase of the DPP project, in which they performed a cross-platform analysis of the digital election landscape in the three of the most popular social media platforms in the Philippines. The data used were public posts from each platform containing election-related keywords from May to October 2021. The researchers pointed to the following as indicators of “networked political manipulation” on social media: The study said that these accounts have contributed to the growth in the influence of politicians in social media, yet they are not necessarily covered by election-related policies. The freedom of these accounts to spread partisan content without the need to disclose their identities has also helped shield them from scrutiny and accountability. These “anti-democratic” actors, as the researchers called them, also often hijacked political discourse on social media by both attacking and copying social institutions like the media. Among the most common tactics of these accounts were baselessly accusing the media of being biased and mimicking the format of news and surveys to feign credibility. The researchers said that the platforms deal with networked manipulation in different ways, but all three have conducted takedowns of inauthentic accounts. Facebook defines it as “ coordinated inauthentic behavior ,” while YouTube characterizes it as “ coordinated influence operations .” Twitter deals with it under its platform manipulation policy. “There are a lot of actions made by the platforms…. But I think, coming from a political-economic perspective, platform commercial interest will always be in conflict with democratic ideals,” Marie Fatima Gaw, a co-lead of the DPP study, said during the presentation. Gaw mentioned Facebook whistleblower Frances Haugen ’s statement on how Meta leaders refuse to make Facebook and Instagram safer even though they know how to, because they prioritize profits before their users. “There are safeguards they can do, but they’re doing it for show somehow. We want to expect more from platforms because they earn a lot from us,” Gaw said. The cross-platform analysis wrapped up the DPP project’s first phase that detailed the Philippine election digital landscape. The first three reports focused on identifying the influential networks of accounts participating in the election discourse on YouTube , Twitter , and Facebook , respectively. The second phase of the project will further flesh out the topics discussed through content analysis, then the third phase will be an in-depth qualitative analysis of the discourse online. The Philippine Media Monitoring Lab is a consortium of researchers in the fields of communication, political science, and data science. The DPP project is co-led by Gaw and Jon Benedik Bunquin, both assistant professors from the University of the Philippines Diliman’s Communication Research department. – Rappler.com How does this make you feel? </t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2022 PH Elections - News,2022 Philippine Elections,digital forensics,Disinformation,social media platforms</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Facebook group sheds Philippine history brand, now spreads Marcos propaganda</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>https://www.rappler.com/philippines/elections/facebook-group-sheds-philippine-history-brand-spreads-marcos-family-propaganda/</t>
+        </is>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>44581.33489583333</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SUMMARY This is AI generated summarization, which may have errors. For context, always refer to the full article. REBRAND. Popular Facebook group 'Philippine History' renames itself to 'BBM Sara at Philippine History' two years after it was first created. Rappler screenshot MANILA, Philippines – The popular Facebook group “Philippine History,” once an online community where members shared nostalgic posts of old Manila and Philippine antiques, has now been rebranded into a space for pro-Marcos propaganda and disinformation. In November 2021, the group was renamed “BBM Sara at Philippine History” so that members could “fulfil their duty as Filipino citizens,” as one administrator said. While administrators used to discourage members from sharing political posts in the group, now they encourage members to “promote [candidates] as [they] see fit.” Even before the group was renamed and repurposed, however, administrators had stated that they were pro-Marcos, but it was rare for them to share posts related to the family. Now that the group has been rebranded, administrators are allowing Marcos propaganda to proliferate and criticize members who do not share the same political views. The group was created in October 2019 and has 542,423 members, as of writing. Members and administrators have shared posts in favor of the Marcoses as well as Sara Duterte, Ferdinand “Bongbong” Marcos Jr.’s running mate in the 2022 elections. Angelo A. Bernardo Jr., who first joined the group around two years ago, recently left due to the influx of posts favoring Marcos and Duterte. “The Philippine History group members then posted a lot of historical articles, photos, memorabilia and articles from the past…. Now it’s mostly Marcos, Duterte posts, with a few historical posts every now and then,” he said. The practice of renaming accounts, pages, and groups with large followings to promote politicians is not new to Filipinos. Rappler readers spotted a number of Facebook pages and groups changing their names to promote possible candidates for the 2022 polls – all done several months before the official filing of candidacies last October. Apart from posts that favor the Marcos family, there are a number of posts in the group – some shared by the administrators themselves – containing false information and misleading content flagged by Facebook and third-party fact-checkers. These include posts about the popular Tallano gold myth and claims that the late dictator Ferdinand Marcos scored 98.01% in the 1939 Bar Examinations, as well as false information on COVID-19 and volcano alert levels . Bernardo said a number of members have also been commenting on different posts complaining about the recent change. Other members tell them they are free to leave the group if they don’t approve of the posts being shared. Even administrators have encouraged critics to leave the group and have kicked out members who share different beliefs. Rappler reported in 2019 about how the Marcos propaganda network on  Facebook has long been seeding false narratives about the family in an attempt to rewrite history. Rappler’s database also monitored several other pages and groups that glorified Marcos Martial Law, some of which had branded themselves as channels that post content related to Philippine history. Some history pages monitored by Rappler explicitly include the Marcos name, and aim to highlight the positive achievements of the late dictator and to promote Marcos Jr. ahead of the 2022 elections. Other history pages and groups in the database did not include Marcos in their display names, but have previously shared posts supporting the family and/or dubious claims about them. These include the group “REAL PHILIPPINE HISTORY” and the pages “REAL Philippine History” and “Philippine History Untold.” Two Marcos history pages on Facebook monitored by Rappler’s tools in 2019 are no longer available, as of writing. Marcos supporter networks have also proliferated on other platforms, such as YouTube , TikTok, and Twitter , with gaps in tech companies’ policies allowing disinformation to thrive. (READ: Anti-disinfo coalition pushes YouTube, Tiktok to crack down on false content ) The Marcoses have burnished their image since they were ousted from Malacañang almost 40 years ago. Marcos Jr. approached controversial political data company Cambridge Analytica to “rebrand” the family’s image, a report that his spokesperson Vic Rodriguez denied. Most recently, Rodriguez also claimed he was unaware of the Tallano gold myth that had made rounds on many social media apps and websites. The myth claims the gold is now with the Marcos family and will be distributed to Filipinos if Marcos Jr. is elected president –  Rappler.com How does this make you feel? </t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>#FactsFirstPH research,2022 PH Elections – News,2022 PH vice presidential race,2022 Philippine Elections,digital forensics,Disinformation,Facebook,Ferdinand Marcos Jr.,Networked propaganda,Sara Duterte,social media platforms</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>The story is not the ‘hack’; it’s the propaganda</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>https://www.rappler.com/plus-membership-program/exclusive-content/story-not-comelec-hack-propaganda/</t>
+        </is>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>44575.41666666666</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SUMMARY This is AI generated summarization, which may have errors. For context, always refer to the full article. Because this is the Philippines, we really shouldn’t think that the official election period would usher in quietly, with a curtain raiser, a calendar story of sorts, doing the trick. The election period started on Sunday, January 9, exactly four months before election day. True enough, even before the week is over, the newsroom has had to be sharper and more discerning in our treatment of several stories. Hello again! I’m Miriam Grace A. Go, the investigative and research head at Rappler. I also set the agenda for our #PHVote coverage. And here I’d like to share how, just as soon as the election period kicked off, we were reminded that the responsible thing for us to do is to not add to the noise and the murk that intensify during this politically-charged season. On Monday afternoon, January 10, the Manila Bulletin ran a story, claiming that the servers of the Commission on Elections (Comelec) were hacked, and that the data downloaded included “information that could affect 2022 elections.” Normally, when another legitimate news site has an exclusive, Rappler doesn’t mind following up on this and crediting the other publication for being first to break the story. Except this “scoop” raised red flags. Comelec itself pointed out loopholes in the Manila Bulletin report, but I’ll share some more reasons Rappler decided to approach the claim with caution: In 2016, Rappler ran stories about the Comelec’s voters database getting hacked because we were able to confirm it independently, having examined the leaked data ourselves. The hackers responsible for it also came forward . (READ: Experts fear identity theft, scams due to Comelec leak ) This time around, with only screenshots available as alleged proof, we agreed with our head of digital strategy Gemma Bagayaua-Mendoza , who said, “reporting on something like this without verifying independently is irresponsible.” This is the link to our story in 2016 where we examined the leaked data. Our report then was not based only on screenshots because reporting on something like this without verifying independently is irresponsible. @paterno_II  https://t.co/5b430LJRWH  https://t.co/3m2NIKrxI7 Besides, the timing of the supposed bombshell was curious, when the spotlight was on Marcos failing – refusing? – to appear before the Comelec to answer petitions to cancel his candidacy or disqualify him. (In case you didn’t know, his lawyer told an infuriated Commissioner Rowena Ganzon that Marcos couldn’t show himself even for a moment in a Zoom hearing because he feared he might spread the virus to other people. Thus, the trending #Zoomicron.) Referring to the hack, Comelec spokesman James Jimenez said: “Because the information was very suss from the very beginning, hindi naman puwedeng basta-bastang dambahan iyong information nila (it’s not right that we just accept their information hook, line, and sinker).” Still, journalists, election watchdogs, and voters themselves should be on the lookout for indications of the election system having vulnerabilities. Or, sometimes, it’s not even the system flaws but how the slightest indication of these are used to feed disinformation. Clearly, there’s another aspect of campaigns and elections that responsible citizens should be watching: propaganda. It spells the difference between informed voters and blind followers, between a credible exercise and one weakened by lingering doubts. How does this make you feel? </t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2022 PH Elections - News,2022 Philippine Elections,Comelec,Networked propaganda</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>[ANALYSIS] Viber: The next frontier for political propaganda in the Philippines?</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>https://www.rappler.com/voices/thought-leaders/analysis-viber-next-frontier-political-propaganda-philippines/</t>
+        </is>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>44549.49818287037</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SUMMARY This is AI generated summarization, which may have errors. For context, always refer to the full article. As is well-known, Facebook is widely used across Southeast Asia, especially in the Philippines, where 99% of internet users have Facebook accounts and 98% use Facebook Messenger , mostly to communicate with family and friends. In comparison, the use of the messaging app Viber is very low – only 5% of internet users use it. However, Viber use is rapidly growing in the Philippines and with it, its political significance grows, too. The Propaganda Lab at the Center for Media Engagement at UT Austin conducted 21 interviews in the Philippines, Indonesia, Myanmar, and Ukraine , and found that Viber is being used for the spread of political propaganda in the Philippines in particular . While Facebook remains widely used for propaganda in Indonesia, for instance, our interviewees in the Philippines articulated that Viber has been “invaded” by Duterte’s government. So, will Viber be the next hotbed of disinformation or misinformation exploited by an authoritarian leader? Disinformation and political propaganda are rampant on Facebook across Southeast Asia but similar phenomena on encrypted messaging applications (EMAs) are underexplored. Apps that use end-to-end encryption (E2E), which tout that only the sender and receiver can see what messages say, are growingly popular across the globe . Troublingly, they are increasingly becoming spaces for mis- and disinformation just like “traditional” social media. They have even led violence to erupt in the offline world, such as mob lynchings in India after disinformation spread on WhatsApp , and played a role in anti-democratic movements, such as the Capitol riot in the United States . The emerging use of Viber, an app that offers E2E in 1-on-1 and group chats (though not in channels or communities) , looks like the next frontier for political propaganda and disinformation in the Philippines and Southeast Asia writ large. For instance, representatives from the Presidential Communications Operations Office interviewed by us explained that the government established Viber groups that include over two million users to distribute information from the government to Filipinos. In addition to government announcements, these groups serve as an avenue to encourage support for President Duterte on a platform that is sure to reach a widespread audience. According to two representatives from the communications office, their goal is to make the president visible – even “ubiquitous.” They aim to make content as entertaining as possible, tailored specifically to younger audiences. One example is sticker campaigns. Graphic designers in the communications department have designed sticker packs with President Duterte’s image paired with politically motivated phrases – people in his office would call this increasing support, but a cybersecurity strategist we spoke to (who is also a former politician), called these “Duterte ads.” He considered these strategies to be more than just spreading presidential news – he explicitly called it “propaganda.” In addition to calculated strategies like sticker packs, government officials thoughtfully select which platforms to engage on as well. “We use Facebook Messenger to blast information to the public.” Although they “try to blast it on all platforms,” they particularly aim to target young folks (millennials and younger) through emerging platforms like TikTok and Viber. This is strategic – the number of TikTok users in the Philippines is increasing , just like Viber. “Filipinos want to go to social media as an escape,” one of the officials told us, “so you must package your content in the most entertaining and trendiest way possible to relate, especially to the millennials.” Their strategies are deliberately coordinated in order to reach the most emerging users. The representatives we spoke to were adamant that such content was not pushed by trolls. “For us, social media is just an additional task of our public information officers.” In fact, a main part of their job description includes content creation and social media management. The creation of in-house social media teams signals how vital social media has become for the Duterte regime. “We don’t hire external outfits or groups to run our social media,” they told us. However, while the people we spoke with who work in Duterte’s communications office would (and did) vehemently deny the use of troll farms, it has been exposed in investigative reporting and academic work alike . The use of Viber differs greatly across different cultures and countries. In Myanmar, for instance, it’s not widely used, and in Indonesia WhatsApp reigns. In general, EMAs are often used to connect individuals into small groups from families to community social groups; with the unintended side effect, however that – “lots of disinformation spreads between family and friends,” as a cybersecurity strategist told us. Hence the additional question arises if Viber will not only be the next outlet for disinformation in the Philippines but also co-opted by troll farms. One man we spoke to in Indonesia (we would refer to him as a troll, but they call themselves “buzzers”) told us about his strategies for political propaganda on traditional social media like Facebook and YouTube: he and his team each run 50 or more accounts, orchestrating fake arguments between the accounts about political candidates. Ultimately, all of the “people” (fake accounts) concede and support the candidate the buzzer/troll was hired to increase support for. This strategy, he told us, is not possible on EMAs. However, he and other interviewees explained that by pushing out positive information about one candidate and negative disinformation about the other, they can still affect public opinion and likely, elections. Ultimately our research has discovered that EMAs are falling prey to exploitation just as other social media sites have. However, there is another side to this challenge, namely the receptiveness and potential engagements of EMA users to disinformation and propaganda. In the Philippines in particular, citizens have been trying to push back against an authoritarian leader – so while online spaces such as Viber and TikTok present opportunities for state actors to manipulate young folks, who are allegedly especially at risk for believing fake news , this research also wants to highlight the opportunities for pushback. For example, EMAs are useful to communicate in private and mock government propaganda or engage in fact-checking to expose government propaganda. For this, researchers must keep a finger on the pulse of disinformation campaigns on emerging platforms since actors, such as the Filipino government, adapt to the ever-changing social media trends for their own goals. – Rappler.com Katlyn Glover is a researcher and graduate student at the Propaganda Lab at the Center for Media Engagement at the University of Texas at Austin, where she researches disinformation and political propaganda on emerging technologies. Zelly Martin Geurink is a researcher and PhD student at the Propaganda Lab at the Center for Media Engagement at the University of Texas at Austin, where she researches disinformation and political propaganda, especially as they pertain to women. How does this make you feel? </t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Disinformation,mobile phone technologies,social media platforms</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>New war: How the propaganda network shifted from targeting 'addicts' to activists</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>https://www.rappler.com/newsbreak/investigative/how-propaganda-network-created-online-environment-justifies-shifted-killing-activists/</t>
+        </is>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>44472.02684027778</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SUMMARY This is AI generated summarization, which may have errors. For context, always refer to the full article. Zara Alvarez served as a human rights defender and paralegal in the Negros islands for Karapatan for more than a decade. She worked tirelessly despite threats and intimidation in a province that’s been witness to decades of war between state forces and insurgents. Alvarez would see her face on posters linking her to the communist underground and she was, in fact, imprisoned for two years. Nothing prepared her for the bloody Duterte years. In 2018, Alvarez was one of 600 activists tagged as terrorists by the Department of Justice. What followed was persistent red-tagging and harassment – she got attacked online and was constantly followed while she worked. Two years later, in August 2020, while walking in the streets of Bacolod City, unidentified men shot Alvarez dead. She was 39. The story of Alvarez illustrates the direct connection between information operations online and physical attacks, a rehash of the government’s war on drugs where supposed drug users and dealers are demonized online to justify attacks against them in the real world. Rappler’s research team found out that from drug war narratives, the focus of government’s coordinated online propaganda network has shifted to red-tagging, which lumps activists with terrorists and turns the communist insurgency into a problem that’s bigger than what it really is. President Rodrigo Duterte himself has enabled this through his speeches and policies. It’s worth noting that prior to the government’s attacks on the Left, Duterte was friends with them for decades – since he was mayor of Davao. The national democratic movement backed his presidential bid in 2016, and after his election, Duterte appointed prominent leftist leaders to his Cabinet. He reopened peace negotiations with the National Democratic Front and declared the longest ceasefire with communist insurgents in three decades. But the talks eventually broke down, as the military gained ascendancy in the Duterte government. By the end of 2017, Duterte’s administration sought to tag more than 600 activists and members of the Communist Party of the Philippines (CPP) as “terrorists.” The list included alleged CPP chairman Benito Tiamzon, Anakpawis chairman Randall Echanis (who would be killed in his home in 2020), ex-Bayan Muna representative Satur Ocampo, and hundreds of John Does . (READ: “ The end of the affair? Duterte’s romance with the Reds ”) To track red-tagging narratives online from January 2016 to August 2021, Rappler used an initial dataset of posts attacking progressive groups and activists on Facebook, plotted an initial roster of red-tagging entities, and used natural language processing to identify keywords commonly associated with the term. These include keywords like “NPA,” “Left Activists,” and “CPP.” The graph above shows a timeline of posts with mentions of keywords typically used for red-tagging from 2016 to 2020. While there have been posts in 2016 and 2017 about the insurgency and military propaganda against the Left, information operations intensified in 2018, when it became clear that the Duterte government was abandoning a negotiated settlement of the insurgency and implementing a militarist approach to crush the guerrillas and their supposed front organizations. In November 2018, for instance, Duterte signed Memorandum 32 that deployed more soldiers and cops in the Negros islands , Samar, and Bicol – known insurgency hotbeds. That same month, Alvarez and the rest of Karapatan-Negros lost a colleague with the murder of human rights lawyer Benjamin Ramos in Kabankalan City. Ramos would be among the first of many Karapatan members and lawyers who would be murdered under the Duterte administration. The following month, in December 2018, the Duterte administration issued an executive order creating a national task force to address the causes of armed conflict with communists at the local level. This task force came to be known as the National Task Force to End Local Communist Armed Conflict (NTF-ELCAC), the main counter-insurgency vehicle that brings together all government agencies for one goal: crush the communists by the time Duterte ends his term in June 2022. “ Doon nagsimula ang malalagim na araw namin (That was when our bloodiest days started),” Clarizza Singson of Karapatan-Negros said as she recounted the incidents between the Sagay massacre in October to the police operations in Guihulngan City in December 2018. Singson had worked with Alvarez for almost a decade before the latter was killed in 2020. These attacks, particularly against Karapatan members, come not as a surprise, considering that the Duterte government and the Philippine military believe that human rights groups are front organizations of the armed movement. As Rappler’s scan showed, the government’s campaign against insurgents was complemented by increased activity online. The biggest surge in red-tagging posts was observed in 2020, as the government deliberated on, and eventually adopted, the Anti-Terrorism Act of 2020 or the Anti-Terror Law . The network map above shows Facebook pages and groups amplifying content related to red-tagging and activism. Pages and groups cluster together when they share content from the same sources. The cluster in blue is the main cluster – mainly pushing out harmful red-tagging content and anti-activist propaganda. Note how the clusters became denser starting in 2018, caused by the increased connectedness of the nodes, showing increased networked behavior. Using natural language processing, we looked at the general themes pushed out by the main red-tagging cluster. The narratives pushed out by the main red-tagging cluster show a focus on creating an enabling environment for violence where activists are painted as “terrorists” and the communist insurgency is a problem bigger than what it is. The tactic is reminiscent of the propaganda playbook for the Duterte administration’s brutal war on drugs and how it justified the killings of alleged drug pushers. (READ: [OPINION] First they came for the pushers and addicts. Now, the Leftists ) While the scan also spotted the usual news reports on civilian-military operations, the bulk of the posts used hateful and harmful language targeting activists and progressive groups. These groups were also frequently tagged as legal fronts of the communist New People’s Army (NPA). Even following her death, Alvarez was not spared from false claims that tagged her as part of the armed movement. Some posts even claimed that the NPA killed her so they could put the “blame [on] the government.” This claim was even echoed by NTF-ELCAC’s former spokesperson Antonio Parlade when he said in a statemen t, posted on NTF-ELCAC’s official Facebook page , that Alvarez “joined the NPA for two years until 2015.” Previous investigations by Rappler show similar demonizing language from dubious, anonymously-managed pages known for perpetuating lies and for red-tagging individuals and groups, amplified by police pages and accounts. (READ: With anti-terror law, police-sponsored hate and disinformation even more dangerous ) Organizations with top mentions in the scan include progressive groups like Bayan Muna, Makabayan, Gabriela, League of Filipino Students (LFS), and Karapatan. There were also significant mentions of state universities like the University of the Philippines (UP) and the Polytechnic University of the Philippines (PUP), which are accused of being “recruitment grounds” for rebels, and a nest for activists-turned-terrorists. On the other hand, groups like the Liberal Party and the CBCP tend to be accused of defending and coddling “terrorists.” Threats and red-tagging often target big progressive voices in Congress, like Kabataan Partylist Representative Sarah Elago and Bayan Muna Representative Carlos Zarate. Akbayan Senator Risa Hontiveros was also often called out for her alleged silence on crimes committed by the NPA. High-profile activists like former Bayan Muna representative Teddy Casiño, as well as celebrity-turned-activist Angel Locsin, were also often targeted and linked to the NPAs. No less than Parlade himself alleged that Locsin’s sister is an NPA – a claim Locsin has consistently denied. And aside from military and NTF-ELCAC spokespersons, the propaganda network would quote “ex-rebels” in their propaganda and red-tagging. These “ex-rebels” are often used to “expose” how rebel recruitment is done in schools, and to supposedly unmask activists who are allegedly members of the armed rebellion. While all these are happening online, activists who are not as popular as the targets of the online information operations are being killed on the ground. Taking from the same tokhang playbook, some police operations that targeted grassroots organizers and local leaders of progressive groups resulted in “ nanlaban” deaths. This included the “bloody Sunday” operations in Calabarzon in March 2021 that left nine activists dead. “ Sanay na kami sa death threat kasi minsan three times a day. Minsan once a week. Minsan once a month…Pero syempre hindi ‘yun empty threats. Pinapatay at namamatay mga kasama ko ,” Singson said. (We are used to death threats. Sometimes, we get it three times a day. Sometimes, once a week or once a month. But these threats are not empty threats. My colleagues are being killed and have been killed.) According to her, they were subjected to surveillance, trumped-up cases, arrests, raids, direct threats, and other forms of harassment. Since Duterte became president in 2016, at least 16 Karapatan members have been killed. They have adjusted by strengthening their security protocols and learning how surveillance works. They employed a buddy system, changed their schedules, and avoided going outside their homes during the day. In Singson’s case, they went as far as abandoning their home and uprooting her whole family – her two young sons included – to live in rented apartments. The slain Alvarez experienced close surveillance. According to Singson, unidentified individuals would openly follow and take photos of her even in public spaces. The necessary adjustments and new security measures disrupted their lives. The tactic of using the drug war playbook against activists seemed to have worked as well. Singson said the way they hid and protected themselves felt like they were being hunted as criminals. “Yung mga bata ayaw namin isubject sa ganung buhay na nanonormalize ang fear, terror, at killings… Para kaming wanted criminal. Daig pa namin ang wanted criminal,” Singson added. (We don’t want to subject the kids to that kind of life where fear, terror, and killings are normalized. We were like wanted criminals.) When Alvarez was gunned down, Singson and her other colleagues in the province received messages from anonymous perpetrators: “You’re next.” Singson fought back against the kind of attacks they experienced. She filed a case at the cybercrime division of the National Bureau of Investigation to track those who, on her Facebook account, threatened to have her head severed. She took screenshots and printed out all the hate messages and death threats she received. But nothing came out of it. According to her, the cybercrime division concluded that the accounts used to attack her were hacked and that was the end of the story. Rappler’s network analysis showed that the online narratives are seeded through a mix of old and new bloggers and “alternative” news sources, with different clusters focused on either funneling to the general public (through hyperlocal and political pages), or niche but engaged communities (e.g., military, police, and their supporters), which become vectors for distribution. At the center of the campaign is the official Facebook page of NTF-ELCAC. Content from other state media like the Philippine News Agency and PTV is also often pushed to spread red-tagging narratives. Previous Rappler investigation has documented how official government platforms, including the hugely-funded NTF-ELCAC , were being used to attack and red-tag local media. (READ: Gov’t platforms being used to attack, red-tag media ) SMNI News, the broadcasting arm of Filipino televangelist and pro-Duterte church leader Pastor Apollo C. Quiboloy, has also been an active source of news content related to the communist rebellion, often shared by the red-tagging cluster. Official military channels are also among top content creators amplified by the cluster, such as the official Civil Relations Service Armed Forces of the Philippines. Army officer Colonel Harold Cabunoc’s Facebook page is also among the most active in creating military and anti-insurgency propaganda. The colonel has also had a history of red-tagging online , and has also been red-tagging slain activists. Other pages shown to be actively pushing out military propaganda are IDOL KU ‘TO, LAMRAG SINIRANGAN, and Pinoy Red Watch. “Alternative” news sources were also actively being funneled by the cluster, including websites pinaslatestnews.xyz, and socialnewstrendph.xqz. These websites post “news” content related to communists, and “report” about government propaganda against activists and progressive groups. Other pages often amplified by the main cluster include known propaganda pages Mocha Uson Blog and VovPH . Content from these sources is shared in hundreds of Facebook pages and groups, mostly political but also including community and interest hubs, with captions that actively call out activists as terrorists, and highlight the narratives identified above. While the main cluster effectively distributes these content to the general public, other clusters showed similar content, also mostly coming from “alternative” news websites and “news aggregators” that are funneled into Facebook groups with special interest in military and anti-insurgency activities, such as Team AFP, Philippine Armed Forces, and the “CITIZENS ANTI-DRUGS CRIMES AND CORRUPTION OF THE PHILS.” While the online and on-the-ground attacks were public and blatant,  support for human rights and progressive groups was muted online. Karapatan secretary-general Cristina Palabay claimed their network and community continuously expanded since 2018 when the attacks against them and other progressive groups increased. “Sa international, after the NTF-ELCAC, dumami rin ang kaibigan namin,” Palabay said. (In the international scene, after the creation of NTF-ELCAC, we gained a lot of supporters.) But this widespread support and network group has yet to translate online. In the digital space, their stories are often told exclusively by select media and the network of progressive groups and human rights activists. The network map above shows the network of pages and groups that amplified content with mentions of 16 Karapatan members killed during the Duterte administration. While progressive groups have their own network of pages and distribution channels, as seen above, they are small in comparison to the red-tagging and propaganda network. In the visualization below, we compare the amplifying agents (Facebook pages and groups sharing their content) of NTF-ELCAC and progressive group Karapatan, as captured by Rappler’s SharkTank in 2020. The two entities were chosen because they were the most distributed content sources for government propaganda and in conversations on activists killed. The scan showed a huge difference in the size of the networks that amplify both channels – painting a picture of an environment where stories of slain activists like Alvarez remain within the echo chambers of other activists online and are effectively drowned out by government propaganda that blurs the lines between activism and terrorism. What makes this enabling online environment more dangerous is how it reinforces the lack of public accountability for the harassment and killings of human rights workers, lawyers, and activists. It also further weakens mechanisms that are supposed to protect individuals who are already vulnerable to attacks such as Alvarez, who asked the Supreme Court for protective writs because she was being harassed. She died before the court came up with a decision on her appeal. – Rappler.com Data visualizations by Akira Medina, Dylan Salcedo How does this make you feel? </t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>activist groups in PH,Disinformation,Facebook,human rights</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Investigating troll farms: What to look out for</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>https://www.rappler.com/newsbreak/iq/investigating-troll-farms-what-to-look-out-for/</t>
+        </is>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>44394.04302083333</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SUMMARY This is AI generated summarization, which may have errors. For context, always refer to the full article. Shutterstock What do people need to watch out for when investigating troll operations? Twelve Philippine senators recently filed a resolution, seeking an investigation into reports that public funds are being used for troll farms. Senate Resolution 768 says Filipinos should know why the national government focuses on spending money on these operations rather than on pressing issues, such as COVID-19 assistance, healthcare, food security, jobs protection, and education. The senators who signed the resolution are Senate President Vicente Sotto III, Senate President Pro Tempore Ralph Recto, Senate Minority Leader Franklin Drilon, and senators Francis Pangilinan, Nancy Binay, Leila de Lima, Richard Gordon, Risa Hontiveros, Panfilo Lacson, Manny Pacquiao, Grace Poe, and Joel Villanueva. Troll farms, the spread of disinformation, and the weaponization of social media are not new to Filipinos. Social media was a key factor in Rodrigo Duterte’s victory in the 2016 presidential polls, and international experts have dubbed the Philippines as “ patient  zero ” when it comes to digital disinformation. The Philippines ranked first in the world for time spent using social media in 2021 , according to We Are Social and Hootsuite’s annual report . This marks the sixth consecutive year the country received this ranking. The senators said the rise in social media and internet usage paved the way for the propagation of internet trolls. If senators will investigate these online operations that spread lies, hate, and disinformation, then here are some of the questions they should ask. What better way to mobilize troll armies than by tapping influential figures or people in positions of power for wider reach? One way the Duterte administration harnesses support for the President is by legitimizing vitriolic attacks on its critics in a bid to control online sentiment. High-profile pro-Duterte propagandists , including Mocha Uson and RJ Nieto , were given government positions or were hired as consultants using public funds. In 2020, Facebook also removed a network of accounts using false identities and which were found to have links to the Philippine military or police . With the anti-terror law , these accounts had been spreading lies and hate against perceived enemies of the State. Celebrities have also been found to be spreading propaganda and fake news, lending legitimacy to questionable sites and fake networks. However, beyond identifying the operators behind these networks, investigators need to ensure these people are held to account. In 2019, Facebook took down a network of accounts that were engaged in inauthentic behavior, and this was traced to Nic Gabunada, Duterte’s social media manager in his 2016 presidential campaign. In June 2021, he was hired by the Department of Finance as a communications strategy consultant. The subject as well as the target of troll army operations can provide more leads on the people behind them. The United States-based network analysis firm Graphika found that the pages involved in Gabunada’s fake network – unsurprisingly – spread pro-government content as well as conspiracy theories about political opponents. In a separate report, Graphika found that a Chinese fake account network had a significant focus on Senator Imee Marcos . Rappler also previously reported on other fake networks supporting the Marcos family , and how widespread disinformation on the Marcoses has attempted to rewrite Philippine history. Most recently, information crowdsourced by Rappler showed Facebook pages and groups as well as Twitter accounts with large followings were renamed to promote potential candidates for 2022. The reports show the practice benefits mostly allies of President Duterte, including his daughter Davao City Mayor Sara Duterte, Cabinet Secretary Karlo Nograles, and Taguig City 1st District Representative Alan Peter Cayetano. The top social media platforms in the Philippines are YouTube, Facebook, Instagram, Twitter, and TikTok. Any of these platforms can be a possible battleground for disinformation operations, especially as the 2022 elections approach. Unclear policies on YouTube , the country’s most popular platform, have resulted in an abundance of false claims on the platform. Videos on Marcos gold claims as well as misleading videos by pro-Duterte vloggers are very common on YouTube. Facebook’s third party fact-checking program does not stop misinformation and disinformation from spreading on its chat app, Messenger. Private messages and channels allow false posts to spread undetected by the platform. – Rappler.com How does this make you feel? </t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Democracy &amp; Disinformation,Networked propaganda</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>How Vietnam's 'influencer' army wages information warfare on Facebook</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>https://www.rappler.com/technology/features/vietnam-influencer-army-force-47-information-warfare-facebook/</t>
+        </is>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>44389.34663194444</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SUMMARY This is AI generated summarization, which may have errors. For context, always refer to the full article. FORCE 47. Sen Hồng or Pink Lotus is among the 'Force 47' state propaganda pages in Vietnam Gelo Gonzales/Rappler In Vietnam, where the state is fighting a fierce online battle against political dissent, social media “influencers” are more likely to be soldiers than celebrities. Force 47, as the Vietnamese army’s online information warfare unit is known, consists of thousands of soldiers who, in addition to their normal duties, are tasked with setting up, moderating and posting on pro-state Facebook groups, to correct “wrong views” online. According to a Reuters review of provincial-level state media reports and broadcasts by the army’s official television station, Force 47 has since its inception in 2016 set up hundreds of Facebook groups and pages, and published thousands of pro-government articles and posts. Social media researchers say the group may be the largest and most sophisticated influence network in Southeast Asia. And it is now playing a prominent role in the country’s intensifying conflict with Facebook. After being approached by Reuters this week, a Facebook source said the company had removed a group called “E47”, which had mobilized both military and non-military members to report posts they did not like to Facebook in an effort to have them taken down. The source said the group was connected to a list of Force 47 groups identified by Reuters. A Facebook spokesperson confirmed that some groups and accounts were taken down on Thursday for “coordinating attempts to mass report content.” A company source said the action was one of Facebook’s largest takedowns initiated under its mass reporting policy. But many of the Force 47 accounts and groups identified by Reuters remain active. Since they are operated by users under their real names, they do not violate Facebook policies, the company source said. Vietnam’s foreign ministry, which handles enquiries to the government from foreign media, did not immediately respond to a request for comment on the takedown. Unlike in neighboring China, Facebook is not blocked in Vietnam, where it has 60 million to 70 million users. It is Vietnam’s main platform for e-commerce and generates around $1 billion in annual revenue for the company. It has also become the main platform for political dissent, launching Facebook and the government into a constant tussle over the removal of content deemed to be “anti-state.” Vietnam has undergone sweeping economic reforms and social change in recent decades, but the ruling Communist Party retains a tight grip over media and tolerates little dissent. Last year, Vietnam slowed traffic on Facebook’s local servers to a crawl until it agreed to significantly increase the censorship of political content in Vietnam. Months later, authorities threatened to shut down Facebook in Vietnam entirely if it did not locally restrict access to more content. In a statement to Reuters, a Facebook spokesperson said the company’s goal was to keep its services in Vietnam online “for as many people as possible to express themselves, connect with friends and run their business.” “We’ve been open and transparent about our decisions in response to the rapid rise in attempts to block our services in Vietnam,” the spokesperson said. Vietnam does not have the wherewithal to sustain a Chinese-style “Great Firewall” and develop local social media alternatives, said Dien Luong, a visiting fellow at the ISEAS-Yusof Ishak Institute in Singapore. “This has paved the way for Facebook to become the platform of choice for Force 47 to safeguard the party line, shape public opinion and spread state propaganda.” There is no official definition of what constitutes a “wrong view” in Vietnam. But activists, journalists, bloggers and – increasingly  –  Facebook users, have all received hefty jail terms in recent years for spreading “anti-state propaganda”, or opinions which counter those promoted by the Party. Last week, Le Van Dung, a prominent activist who regularly broadcasts live to thousands of followers on Facebook, was arrested after more than a month on the run, according to a police statement. Dung, who goes by “Le Dung Vova” was detained on charges of “making, storing, spreading information, materials and items for the purpose of opposing the state,” under Article 117 of Vietnam’s Penal Code. He faces up to 20 years in prison if found guilty. Force 47 takes its name from Directive 47, a policy document issued by the army’s General Political Department on January 8, 2016. Analysts say it was created as an alternative to hiring civilian “opinion shapers” – or “du luan vien” – that had operated on a smaller, less successful scale. “Since the ‘du luan vien’ were not as well trained in Party ideology or as conservative as military officials, their performance was not as good as expected,” said Nguyen The Phuong, a researcher at the Saigon Center for International Studies. “Force 47 is also less costly. Military officials consider it part of their job and don’t ask for an allowance.” The size of Force 47 is not clear, but in 2017, the general in charge of the unit at the time, Nguyen Trong Nghia, said it had 10,000 “red and competent” members. The true number could be much higher: the Reuters review of known Force 47 Facebook groups showed tens of thousands of users. The Facebook source said the E47 group it had taken action against was made up of an active membership of military and non-military members. Nghia now heads the main propaganda arm of the Party. Vietnam’s information ministry recently promulgated a social media code of conduct that closely resembles Force 47 directives, urging people to post about “good deeds” and banning anything that affects “the interests of the state.” In March, conferences were held at military bases across Vietnam to mark five years since the creation of Force 47. State media reports about the meetings named at least 15 Facebook pages and groups it said were controlled by Force 47 which collectively had over 300,000 followers, according to a Reuters analysis of those groups. Rather than being a single army unit, Force 47 soldiers appear to carry out their activities alongside their usual duties and create locally targeted content, the reports revealed. In addition to Facebook, Force 47 creates anonymous Gmail and Yahoo email addresses, and accounts on Google’s YouTube and Twitter, according to the reports. YouTube said it had terminated nine channels on Friday for violating its policies on spam, including a channel identified by Reuters as a suspected Force 47 operation. Twitter said it had not seen any activity by Force 47. Many of the Facebook groups reviewed by Reuters played on patriotic sentiments with names such as “I love the Socialist Republic of Vietnam”, “Vietnam in my Heart”, “Voice of the Fatherland” and “Believe in the Party”. Some groups, such as “Keeping company with Force 47” and “Roses of Force 47” were obvious in their affiliation, while others – such as “Pink Lotus” and a few groups that used the names of local towns in their titles – were more subtle. The posts varied in content, with many extolling Vietnam’s army, founding leader Ho Chi Minh, or Party chief Nguyen Phu Trong. Others showed screenshots of “wrong information” posted by other Facebook users, marked with a large red “X”. “These developments unfolding in Vietnam are scary and have expanded with impunity,” said Dhevy Sivaprakasam, Asia-Pacific policy counsel at internet rights group Access Now. “We are witnessing the creation of a reality where people are not safe to speak freely online, and where there’s no concept of individual privacy.” – Rappler.com How does this make you feel? </t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Disinformation</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Duterte wants vaccine deniers arrested | Evening wRap</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>https://www.rappler.com/video/daily-wrap/june-22-2021-evening-edition/</t>
+        </is>
+      </c>
+      <c r="D17" s="2" t="n">
+        <v>44369.56296296296</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Today on Rappler – the latest news in the Philippines and around the world: President Rodrigo Duterte on Monday, June 21, threatens to arrest Filipinos who refuse to get vaccinated. President Rodrigo Duterte calls the International Criminal Court ‘bullshit,’ a week after the body’s chief prosecutor recommended opening a formal investigation into his drug war. The Department of Finance defends its hiring of Nicanor Gabunada Jr., a public relations practitioner tagged by Facebook as the operator behind a fake news, pro-Duterte propaganda network. Hong Kong leader Carrie Lam hits back against critics of the Chinese territory’s attacks against pro-democracy tabloid Apple Daily. The future looks bright for the all-cadet Gilas Pilipinas after it wraps up the FIBA Asia Cup Qualifiers without a loss. – Rappler.com How does this make you feel? </t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>COVID-19 vaccines,Department of Finance,FIBA Asia Cup,Hong Kong,Hong Kong Security Law,International Criminal Court,Networked propaganda</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>The fake social media accounts amplifying Chinese propaganda</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>https://www.rappler.com/technology/features/pro-china-fake-social-media-accounts-coda-story/</t>
+        </is>
+      </c>
+      <c r="D18" s="2" t="n">
+        <v>44340.38846064815</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SUMMARY This is AI generated summarization, which may have errors. For context, always refer to the full article. Teona Tsintsadze for Coda Story An army of suspicious “super-spreader” social media accounts stationed around the world is helping Chinese diplomats amplify the country’s perspective on current events, according to a new investigation. The findings of seven months of research were published in a study by the Oxford Internet Institute last week, analyzing every tweet and Facebook post by Chinese diplomats and 10 of the nation’s largest state-controlled media outlets between June 2020 and January 2021. The researchers examined 189 accounts attributed to China’s embassies, ambassadors, consuls, and other embassy staff. It discovered an extraordinarily high level of engagement on social media: Chinese diplomats tweeted 201,382 times, averaging 778 times a day for a nine-month period. Their posts were liked nearly seven million times and retweeted 1.3 million times. Many of the shared posts helped amplify content from China’s state-backed media, enabling the diplomats to act as bridges between state media and local communities. The investigation has also found evidence showing that social media audiences engage with Chinese diplomatic Twitter accounts in large numbers. Chinese diplomatic accounts were retweeted more than 735,664 times between June 2020 and January 2021. Moreover, this engagement is dominated by a small number of “super-spreader” accounts, which rapidly engage with content posted by Chinese diplomats. At least 270 Chinese envoys in 126 countries are active on Twitter and Facebook. In a separate collaboration with the Associated Press, Oxford Internet Institute researchers uncovered evidence of a pro-China amplification machine based in the U.K., with a coordinated inauthentic network of 62 accounts dedicated to promoting content by Chinese diplomats stationed in London. Between June 2020 and January 2021, it accounted for nearly half of all retweets of China’s ambassador to the U.K. “The network nearly doubled the ambassador’s retweet counts, lending him a false sense of popularity and artificial support, which may make his positions seem more credible,” said Marcel Schliebs, the report’s lead researcher. Many of the accounts impersonate British citizens by claiming they support football clubs in London or Manchester, and frequently use language suggesting they are U.K.-based. While some accounts showed obvious signs of coordination, the researchers said they could not definitively conclude whether the 62 in question were controlled by one or more operators. While Twitter last year disclosed the takedown of nearly 29,000 accounts linked to a China-backed information campaign between August 2019 and June 2020, the process can take months. “Twitter should establish clear criteria of what constitutes coordinated inauthentic behavior and monitor accounts with suspicious engagement more closely,” said Schliebs. In response to the Associated Press findings, the Chinese embassy in London said it was aware of concerns about posting on Twitter. “If it is against the rules of social media to retweet the Chinese embassy’s tweets, then shouldn’t these rules be more applicable to retweets of malicious rumours, smears and false information against China? We hope relevant companies will not adopt double standards,” it said in a statement. – Rappler.com Ramsha Jahangir is an award-winning journalist at Pakistan’s DAWN newspaper. She covers technology, human rights, disinformation and digital politics. This article has been republished from Coda Story with permission. How does this make you feel? </t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>China</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>WATCH: How the propaganda machine took a beating when #OustDuterteNow trended</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>https://www.rappler.com/philippines/video-how-propaganda-machine-took-beating-oust-duterte-trended/</t>
+        </is>
+      </c>
+      <c r="D19" s="2" t="n">
+        <v>44041.41827546297</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Analysts say the Duterte administration’s response to the raging health crisis carries a high political cost. The outbreak hits several of the President’s main constituencies in both the middle class and overseas Filipino workers. Ateneo School of Government Dean Ronald Mendoza says that if government is unable to respond effectively, “we may witness change in political support.” Another analyst, University of the Philippines political science professor Ela Atienza, says Duterte and his team may have touted the war on drugs, massive infrastructure programs, and development in regions outside Metro Manila as legacies of his administration, but it’s clear the pandemic “has changed the agenda for the rest of his term.” Watch this video and find out how Rappler documented the beating that the propaganda machine took at the hands of unaligned, unpoliticized individuals. Data shows the #OustDuterteNow trend was largely organic and participatory, with little signs of manipulation or coordination. This pointed to a groundswell of negative public sentiments against the President’s handling of the crisis. – Rappler.com How does this make you feel? </t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Duterte Year 4,Rodrigo Duterte</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Duterte’s troll armies drown out COVID-19 dissent in the Philippines</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>https://www.rappler.com/technology/features/philippine-troll-armies-coda-story/</t>
+        </is>
+      </c>
+      <c r="D20" s="2" t="n">
+        <v>44034.33354166667</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SUMMARY This is AI generated summarization, which may have errors. For context, always refer to the full article. Visuals by Sofiya Viznaya for Coda Story On a sweltering Monday morning in Manila, Nic Gabunada is sitting at his laptop, working from home. Gabunada is a former CEO of Omnicom Media Group Philippines and currently executive director of his own communications and marketing company. Before this, he served for two years as the head of President Rodrigo Duterte’s social media team and played an integral part of his 2016 election campaign. In March 2019, Gabunada was linked to a network of 200 pages removed by Facebook for “coordinated inauthentic behaviour.” This opaque charge is most commonly levelled by the company at foreign influence and troll campaigns. So far, Gabunada is the only individual to have ever been named by the platform as the organizer of such an operation. Despite the actions against his network, Gabunada’s methods have changed politics in the Philippines, where troll farms continue to churn out pro-government messages and attack opposition figures. What is more, Gabunada believes that global platforms face a losing battle in trying to stem the spread of fake news. “No one can control what people can say on social media,” he told me, during a telephone conversation. This is a particular concern during a global health crisis. As Covid-19 has rampaged across the globe, so too have anti-science narratives and conspiracy theories related to the virus. The Philippines has reported 21,895 confirmed cases of coronavirus and 1,003 deaths, so far. The government’s handling of the situation has split the population and online discourse has become increasingly heated, with wild accusations and threats of violence made, often using troll accounts. “Right now in the Philippines – we see offensive posts from both sides,” said Gabunada, referring to the deluge of relentless vitriol raging between pro and anti-Duterte supporters on various social media platforms on a daily basis. “There are newly created accounts on Facebook and Twitter participating in the exchange around the government’s Covid-19 response, but they still belong to one of two sides of the debate – anti or pro.” Amidst one of the longest lockdowns in the world, Gabunada, like many of Manila’s 12.5 million inhabitants, watches all of this from home quarantine. As a healthy distraction, he has taken up kitchen gardening, growing vegetables at home. As the coronavirus continues to plague the Philippines – the country’s health ministry recently reported its fifth straight day of over a thousand infections – the government has moved to silence all criticism. A new anti-terrorism bill which took effect last week has been singled out by rights groups who say it could give the president unprecedented power to target dissent rather than terrorism. The bill permits warrantless arrests and allows authorities to detain individuals for weeks without charge, surveillance for up to 90 days and mandates punishment as severe as lifetime imprisonment without parole. At least nine petitions to revoke parts or the entirety of the law have been filed in the supreme court. The new legislation follows a crackdown on the media’s ability to report on the government. In June, Maria Ressa, founder and executive editor of the news website Rappler, and a former colleague were convicted of cyber libel over a 2012 story that alleged drugs and human trafficking links between a businessman and a top judge by a court in Manila, a charge that they both deny. Both have been fined $8,000 and could now face up to six years in prison. Against this backdrop of repression, Duterte and his administration freely spread political and medical disinformation to Filipino citizens. In early February, the country recorded the first Covid-19 death outside China. The president’s reaction was to hold a press briefing, in which he assured everyone that the pandemic would “die a natural death, even without vaccines.” The following month, however, he delivered an impromptu national address, in which he told police to kill quarantine violators. “My orders to the police and military,” he said, “If there is trouble or the situation arises where your life’s on the line, shoot them dead.” As the crisis has played out, social media posts in support of his confused approach have become increasingly visible. Twitter accounts have been posting pro-Duterte propaganda, including lauding him for his “humility, respect, and gratefulness” and praising the anti-terrorism bill . While many of the tweets appear to be the product of troll operations or bots, Gabunada maintains that the proliferation of pro-government social media hashtags are from legitimate supporters of Duterte. “It is the nature of social media to encourage sharing of opinions and messages,” he said, by way of explanation. However, in April, Twitter suspended hundreds of accounts tweeting under specific hashtags defending the Philippine government’s response to the coronavirus pandemic . According to the Washington Post, the accounts were “posting duplicate content across multiple accounts, creating duplicate or multiple accounts, and sending large numbers of unsolicited replies or mentions.” Most of the accounts posting pro-Duterte hashtags had “suspicious elements” such as bot-like numbers on Twitter account names and few followers. Many users were also new, with the accounts created in March or April. Earlier this month, Facebook released a statement, saying that it was looking into “reports of suspicious activity” in the Philippines, after students, journalists and opposition figures found a deluge of impostor accounts made under their names prompting an investigation by government agencies. While the imposter accounts have yet to publish any posts, opposition senator Francis Pangilinan said he suspected the accounts targeted those who oppose Duterte’s anti-terror bill. The weaponizing of social media can be traced back to the election in 2016. A 2017 Oxford University study found that Duterte spent $200,000 to hire up to 500 trolls during his presidential campaign the previous year. His social media strategy was overseen by Gabunada, who was working as a private contractor. According to Gabunada, Facebook became a cheap and convenient vehicle for the Duterte campaign when the platform struck deals with local cellular operators, making it free to use in the Philippines for anyone with a smartphone. Now, the Philippines has become home to hundreds of troll farms. In March, Reporters Without Borders released a study that explained how supporters of the president acting as “cyber-troll armies” are using “call center hubs” to disseminate “fake or maliciously edited content” and to conduct “targeted harassment campaigns” against opposition figures. A NATO report published earlier this year found that troll farm employees can earn up to $1,000 per month working on political campaigns. The average monthly salary in the Philippines is $278 per month. In an effort to maintain distance from political figures and parties, these operations are also run by private contractors hired by political candidates. But Gabunada says that the 2016 campaign also saw the rise of an online army made up of genuine Duterte supporters. “At the end of the day, you wanted to convert people into campaigners and voters. Fake accounts can’t vote and paid trolls may not necessarily be there when a campaign needs to mobilize them,” he explained. “We organized a network of volunteers to campaign and then we programmed a series of messages to post and amplify on social media accounts. We communicated with these organized groups and encouraged them to create their own Facebook groups and pages – all carrying the Duterte messages and getting as many within their circle to join them.” Pro-Duterte troll farms have lately come up against a growing number of fact-checking groups and ordinary Filipinos dedicated to debunking misleading claims. Jecon Dreisbach, 24, is a former volunteer at a fact-checking organization named the Consortium of Democracy and Disinformation. Today, he works as an independent researcher and educator, specializing in issues of nationalism, politics and the media. One of the biggest fake stories he has recently uncovered involved an April 2020 report by the Philippine News Agency that claimed “80% of Filipinos are satisfied with the government’s response to Covid-19.” The piece cited a survey conducted by a fake polling company based in Bulgaria. Vietnam is economically less-fortunate than the Philippines. Yet, they didn't enforce oppressive policies. What did they do? Enforce public health drives such as coming up with free disinfectants for everyone, among other things. Life went on. Dito? De facto martial law. For their efforts, activists such as Dreisbach frequently become the targets of coordinated online harassment campaigns. “Whenever my criticisms of Duterte go viral, I get trolled,” he said. One notable post threatened Dreisbach with a lawsuit, stating that his fact-checking work was “instigating people to overthrow the government during a state of public emergency.” Matagal ko nang alam na iyong posts ko ay archived na sa pro-Duterte (Youth) Google drive. Kung may mangyari man sa akin, hanapin niyo ako sa lahat ng kampo ng pulis at militar. Hindi ako natatakot sa inyo. Patuloy kong ipaglalaban ang mga pinahirapan at ginutom ng rehimeng ito. pic.twitter.com/dwk4QaH4rF And that is not the worst of it. On May 13, a Duterte supporter posted a tweet threatening to cut off the head of journalist Barnaby Lo. Lo notified the Philippines’ National Bureau of Investigation, but so far the case has not been pursued. While acknowledging that the Philippines is “at a critical juncture in its political history,” Dreisbach remains surprisingly stoic. “It is my constitutional right to express my opinions against the Duterte regime,” he told me. To everyone who stood up for me after someone threatened to cut my head off… The NBI did respond, but said they’re busy w/ child cybersex cases now. I also got a half-apology👇. I realized there are bigger injustices, so I’ve decided not to pursue my complaint. Thanks guys! https://t.co/NK58w3nUqU  pic.twitter.com/hArnQnkjPU Dreisbach also believes that the tide is turning. He largely attributes this change to the government’s handling of the coronavirus and its aggressive use of online platforms to spread misinformation and silence opposition voices. “I am hopeful that Filipinos will be more critical of the policies and disinformation propaganda implemented by the regime,” he said. “Duterte may take advantage of the vulnerabilities we experience in this pandemic to advance his authoritarian desires, but the sovereign Filipino people will march for their fundamental human rights and justice.” – Rappler.com Lynzy Billing is a journalist and photographer based between Afghanistan and the Philippines.  This article has been republished from Coda Story with permission.  How does this make you feel? </t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Networked propaganda</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Gov’t platforms being used to attack, red-tag media</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>https://www.rappler.com/newsbreak/investigative/260602-government-platforms-being-used-attack-red-tag-media/</t>
+        </is>
+      </c>
+      <c r="D21" s="2" t="n">
+        <v>43963.20050925926</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Supposedly at the helm of the Presidential Task Force on Media Security, the PCOO reposts misleading content against media from an anti-communist government page     MANILA, Philippines – Official Facebook pages of the Duterte government shared content that targeted local media just a week after the celebration of 2020 World Press Freedom Day. But this is not the first time verified government pages have done this.  On May 8, the Facebook page of National Task Force to End Local Communist Armed Conflict (NTF-ELCAC) posted a series of infographics that incorrectly said media giant ABS-CBN’s franchise was not renewed because “they have issues with the law.” (READ:   EXPLAINER: FICTAP Issues vs ABS-CBN’s franchise renewal   )   A few hours later, it shared another post that accused Rappler CEO Maria Ressa of spreading "fake news" in her interview with ABC News where she mistakenly said that ABS-CBN has 11 million workers instead of 11,000. Ressa   explained that it was a slip of the tongue: "my mind raced ahead to the market cap ... which was in hundreds of millions of dollars."  She   apologized   for the error. (READ:   NTF-ELCAC 'black propaganda' vs Maria Ressa, ABS-CBN sparks outrage   )   NTF-ELCAC’s posts were shared by the verified pages of the Presidential Communications Operations Office (PCOO) and Radio Television Malacañang (RTVM) just hours after they were posted.  Journalists, academics, and media groups condemned this behavior and called it “black propaganda offensive.” They said it's an abuse of authority on the part of NTF-ELCAC that willfully endangers ABS-CBN's workforce and Ressa. (READ: Media, academics condemn NTF-ELCAC's attacks vs ABS-CBN and Maria Ressa ) This also shows how government is using its platforms, massive resources, and public funds to hit back at critics and perceived enemies.  ‘Crossposting’ of content   By sharing NTF-ELCAC’s posts against ABS-CBN and Ressa, PCOO and RTVM amplified its reach from thousands to millions. More importantly, it linked legitimate concerns regarding press freedom in the Philippines with the government's war against communist rebels.   The NTF-ELCAC page has 25,246 followers and 23,779 likes as of writing. In comparison, the official PCOO page has over 2.1 million followers and 1.7 million likes, while RTVM has 239,000 followers and 159,000 likes.   Though the posts against ABS-CBN and Ressa have since been taken down by the 3 pages, the government has yet to apologize for the incident. The attacks by these government pages have already spread and done damage difficult to rectify.  On May 9, both Presidential Spokesperson Harry Roque and PCOO Secretary Martin Andanar disowned NTF-ELCAC’s posts and said that it was not the official position of their offices.  Like the Office of Presidential Spokesperson (OPS) and PCOO, the NTF-ELCAC is under the Office of the President. It also has a member from the PCOO: Undersecretary Lorraine Badoy, who serves as its spokesperson.  Outspoken against Duterte critics, Badoy previously called research outfit Ibon Foundation a communist front and tagged a number of activists as ranking members of the CPP-NPA-NDFP . She had been previously called out for posting inaccurate claims on her social media accounts. On May 11, following a backlash, Andanar released Department Order No. 20-009 which limits crossposting , or sharing other pages’ content, on the PCOO Facebook page. The department order said that only the livestreams of news events and briefings of President Rodrigo Duterte, Chief Legal Counsel Salvador Panelo, Roque, and its attached media agencies shall be crossposted on the PCOO page. Andanar also said they have identified the individual who crossposted NTF-ELCAC’s content on PCOO’s page but did not name who was responsible. He vowed proper action will be taken and that the office will “uphold accountability on matters like this in order to minimize such unfortunate instances from happening again in the future.” In the past, the official pages of PCOO, RTVM, and NTF-ELCAC had repeatedly amplified each other’s posts. When sharing each other's content, these 3 pages always crossposted within the same day they were originally posted.  From July 2018 up to April 2020, these 3 pages shared each other’s content at least 35 times – not including the posts that have been taken down. RTVM posts were shared the most by the two pages.           Meanwhile, RTVM and PCOO just started sharing NTF-ELCAC’s posts fairly recently – starting in April 2020. Out of the 4 crossposted content from NTF-ELCAC, two mentioned a media organization.   The first one called out Inquirer.net for allegedly publishing a story that “misleads the public,” while the other post shared photos of online news magazine Pinoy Weekly and tagged it as “propaganda materials.” NTF-ELCAC shared on April 20 both posts about the   arrest of Anakpawis volunteers   while they were on the way to a relief operation in Norzagaray, Bulacan.  The table does not include the posts against ABS-CBN and Ressa because they were already taken down as of writing. However, based on screenshots, it was also evident that both PCOO and RTVM shared NTF-ELCAC’s posts within 24 hours.     Screenshots from PCOO and RTVM Facebook page  Red-tagging, disinformation   NTF-ELCAC was established through Duterte’s   Executive Order (EO) No. 70   . The task force “aims to implement an efficient mechanism and structure for the whole-of-nation approach to realize the aspiration of the Filipino people to attain inclusive and sustainable peace.”   The Facebook page of NTF-ELCAC was created on November 4, 2019. Its posts vary – from government advisories, anti-communist advisories, and Duterte administration accomplishments, to warnings against the spreading of false information on social media.   In May 2020, however, it started posting content against the renewal of the ABS-CBN franchise. When asked why an anti-communist task force was posting content about ABS-CBN, it claimed that the issue is being used by the Left “to sow chaos and agitate and divide the Filipino people,” PCOO Undersecretary Badoy said.  The Supreme Court defined red-tagging as “the act of labeling, branding, naming and accusing individuals and/or organizations of being left-leaning, subversives, communists or terrorists (used as) a strategy…by State agents, particularly law enforcement agencies and the military, against those perceived to be ‘threats’ or ‘enemies of the State.’” (READ: Lives in danger as red-tagging campaign intensifies ) Using data captured by Sharktank, Rappler’s own social media monitoring tool, we found that the posts of NTF-ELCAC were also often amplified by pages known to post content that red-tags progressive groups and individuals. The visualization below shows how NTF-ELCAC is connected to the Facebook pages and groups that systematically share each other's content. (NTF-ELCAC is the red node at the lower right side.)  If an arrow from node A points to node B, it means node B shared content posted by node A. The bigger the node and the circle, the more engagements it received within the network. Sharktank identified two amplifiers of NTF-ELCAC’s posts that had previously shared content linking individuals and groups to communist organizations in the country: WeSupportAFP and PNP.TagapagUgnay (PNP Police Community Relations Group-PULISerbis). These pages shared NTF-ELCAC’s posts at least thrice from July 1, 2019 to April 22, 2020. These pages are connected to an even larger network of accounts that systematically propagate each other's content. Click on the circles to see each channel’s name, URL, and how they are connected to other channels. Rappler fact checked a post originally published by PNP.TagapagUgnay, a page officially operated by the Philippine National Police (PNP), which falsely claimed that Kabataan Partylist representative Sarah Elago called for people power in relation to the enhanced community quarantine in late April 2020. The page has since deleted the post. The PNP said it will investigate the matter but has yet to give an update on the investigation. Other pages within this network also published this false claim.  Meanwhile, NTF-ELCAC often shared content from other official government websites such as PNA and PIA. It also amplified posts of the Facebook page of the National Security Council and Kalinaw News, the Facebook page of the Philippine Army’s online news platform.   The latest   State of Media Freedom in PH   report from the Freedom for Media, Freedom for All (FMFA) Network said red-tagging is one of the tactics used by the Duterte administration to stifle the media.   FMFA’s report explained that on the ground, the National Intelligence Coordinating Agency has been holding forums for members of the community media in regions where journalists were “compelled” to sign off to a “Manifesto of Commitment” to declare their support for the implementation of Duterte’s EO No. 70.   If they declined, the report said, it would have been seen as an act of defiance. (READ:   Press freedom takes a hit in PH during coronavirus pandemic   )  There had been incidents, too, where members of the media were publicly linked to the Communist Party of the Philippines (CPP), the New People’s Army (NPA), or the National Democratic Front (NDF). (READ:  Altermidya correspondent, 4 human rights leaders arrested in Tacloban  )  On January 25, NTF-ELCAC posted a quote card of Badoy linking columnist Tonyo Cruz to the CPP-NPA-NDF. The quote was lifted from an article she wrote for PNA that was published the same day.   A history of attacks against media  The PCOO is supposed to be at the helm of the Presidential Task Force on Media Security, a task force mandated to ensure the safety of journalists in the country. But NTF-ELCAC’s posts were not the first time a government agency used its official platforms to target members of the media.  In 2017, the official Facebook page of the Office of the Presidential Spokesperson (OPS)   posted a negative comment   targeting journalists during a livestream of a briefing attended by media.    Screenshot of OPS statement   The comment, which insulted a certain Pia (not clear whether Rappler’s Pia Rañada or ABS-CBN’s Pia Gutierrez) and Lourd Devera (Lourd de Veyra) was later taken down. Malacañang said the comment was posted by someone no longer connected with the OPS, but it did not apologize for the incident. (READ:   Presidential Spokesman Facebook account posts troll-like comment   )   In 2019, blogger Mark Lopez   went on Radio Pilipinas   , a radio station owned by the Philippine Broadcasting Service under the Presidential Communications Group, to call for a protest against Rappler.   Mocha Uson, who has been appointed twice by Duterte – as PCOO assistant secretary in 2017 and again as deputy executive director of the Overseas Workers Welfare Administration in 2019 – has also repeatedly used her platform to push negative posts about the media.   Uson was the first to aggressively push the term “presstitute,” a derogatory term for members of the media who are critical of Duterte. Uson’s page has millions of followers. (READ:   Press freedom after 2 years of Duterte   )   Worrisome state of press freedom   In 2020, the Philippines ranked two places lower at 136th out of 180 countries on the Reporters Without Borders' (RSF)   World Press Freedom Index   .   The report said two factors that pushed down the country’s rank was its state troll armies that   weaponize disinformation   on social media, and its intolerance of critical journalism. (READ:   Philippines slips 2 places in World Press Freedom Index   )   Intimidation, arrests, and murders of journalists in the country have also remained rampant, according to   FMFA’s report   . From January 1, 2019 to April 30, 2020, there were 61 reported incidents of threats and attacks against the media, including 3 journalists who were killed. Thirty of the 61 incidents were allegedly done by state agents.   When state powers wage a propaganda offensive against members of the media, this stifles the people’s right to a free press, which, in turn, threatens a working democracy.  – with Gemma Bagayaua-Mendoza and Loreben Tuquero/Rappler.com  </t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Coronavirus response: Online outrage drowns out Duterte propaganda machine</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>https://www.rappler.com/newsbreak/in-depth/coronavirus-response-online-outrage-drowns-duterte-propaganda-machine/</t>
+        </is>
+      </c>
+      <c r="D22" s="2" t="n">
+        <v>43945.38333333333</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SUMMARY This is AI generated summarization, which may have errors. For context, always refer to the full article. Against the royal blue and rich red of the Philippine flag, President Rodrigo Duterte stood behind a podium bearing the presidential seal, eyes focused on the camera as its lens zoomed in slowly, closing in for a tighter shot. Frustrated over the events that took place on April 1 in Quezon City, a sudden announcement was given at past 9:30 pm, that the Chief Executive was to give a speech. Less than 10 minutes after the notice was sent to media, Duterte appeared on Filipinos’ screens to deliver a stern warning. A furious Duterte said he would not hesitate to take action following the arrest of 21 Quezon City residents who were apprehended for demanding government help and protesting without a permit. The protest, which Duterte accused lefitst group Kadamay of instigating, had manifested weeks of mounting desperation spurred by the government’s slow response to aid residents who were left hungry and out of work due to the lockdown in Luzon. Lashing out at the Left, the President warned they would be detained. Then he took it a notch up. “ I will not hesitate. My orders are sa pulis, pati military, pati mga barangay na pagka ginulo at nagkaroon ng okasyon na lumaban at ang buhay ninyo ay nalagay sa alanganin, shoot them dead ,” he said. “ Naintindihan ninyo? Patay. Eh kaysa mag-gulo kayo diyan, eh ‘di ilibing ko na kay o,” Duterte said. (I will not hesitate. My orders are to the police and military, also the barangay, that if there is trouble or the situation arises that people fight and your lives are on the line, shoot them dead. Do you understand? Dead. Instead of causing trouble, I’ll send you to the grave.) Outrage over Duterte’s remarks was swift. Social media timelines flooded with users who were shocked and angered over the President’s remarks, calling for his ouster. By his next address two days later on April 3, Duterte claimed he hadn’t issued a “shoot to kill” order. “ I never said in public shoot to kill, period. Sinabi ko…if you think that your life is in danger, maging biyuda ang asawa mo na maganda, mag-asawa uli, at ang mga anak mo mawalaan ng tatay, ‘pag tiningnan mo na delikado ang buhay mo, patay, unahan mo na, patayin mo ,” he said. (I never said shoot to kill, period. I said…if you think that your life is in danger, your beautiful wife will become a widow, marry again, and your children will become fatherless, if you think your life is at stake, kill, go ahead, kill them.) He then directly addressed the calls for his ouster. “ Bakit pa ako magpayag na magbarilan tayo? Kaya ganun. Huwag na ‘yang ‘Oust Duterte’ na mga fake news ,” he said. (Why would I allow us to shoot one another? So there. Never mind that ‘Oust Duterte’ that’s fake news.) But by then, widespread online protest had already taken place. Outrage over Duterte’s remarks were widespread with #OustDuterteNow trending worldwide with almost 500,000 tweets. To see how the public responded to the President’s speeches online, Rappler’s data team collected a sample of 15,000 tweets with mentions of Duterte and related words from March 30 to April 2, 2020, and clustered these according to topic using natural language processing. Compounded with analysis from US-based Graphika that dove into the specific hashtags that trended, the data shows that these critical movements were not only large but organic – flooding out even the administration’s supporters known for their coordinated campaigns to mob critics and whitewash the government’s lapses on social media. While critical tweets against Duterte and his administration peaked on April 1, frustrations were already boiling from March 30, when he addressed the nation to give updates on the government’s COVID-19 response. It was the first Monday after Duterte signed a law granting himself special powers to contain the spread of the virus. Filipinos were told to expect a message from the President tentatively set at 4 pm. Filipinos waited for an hour, and then another, and then 5 more. It was past 11 pm when Duterte’s message went live on their screens. “ May mga doktor na, mga nurses, attendants, namatay. Sila ‘yung nasawi ang buhay para lang makatulong sa kapwa. Napakasuwerte nila. Namatay sila para sa bayan ,” Duterte said early into his pre-recorded address. (There are doctors, nurses, attendants who died. They were the ones who died helping others. They are so lucky. They died for the country.) The statement, intended to praise health workers who have risked their lives, quickly drew backlash both online and in the front lines of the outbreak. Doctors, nurses, and health workers did not need the sort of “praise” from the President, Mikey*, a doctor at a coronavirus designated hospital told Rappler. “I’m doing this because it is my duty, but I did not sign up to die,” she said. “I don’t want to die.” Online, Duterte’s remarks drew fierce criticism with many users pointing out doctors died due to inadequate protection and the government’s failure to provide life-saving protective equipment early on in the outbreak. Like other speeches, the President’s remarks targeted critics and focused on threats, instead of facts and concrete plans on the outbreak. Filipinos once again took to social media to express their anger at the government’s handling of the crisis. Rappler found that the two speeches on March 30 and April 1 made for the core of online conversations on Duterte. Tweets were largely critical of the Duterte administration, with the one of the largest clusters hitting the President’s remarks on how health workers are “lucky to die” for the country. Filipino Twitter called the President out, saying he “should not romanticize their deaths” and that the remarks were “insensitive” to medical workers who risked their lives. On the sidelines are criticisms on other fronts. As early as 6 pm on March 30, #DuterteStandardTime trended on Philippine Twitter as people waited for the Duterte speech broadcast 7 hours late. Online users criticized his tardiness at such a crucial time, calling it a trend for the President. “As both head of state and head of government, the President is expected to not only provide direction and lead government but also provide a sense of unity among citizens, particularly during periods of crisis,” University of the Philippines Political Science professor Ela Atienza said. She added, “Unfortunately, President Duterte’s statements, timing of public statements, and style of delivery have not provided reassurance and trust in government.” Public sentiment manifested this as others online also criticized the lack of concrete plans in his speeches. With Filipinos halfway into the lockdown first set to end on April 12, the public demanded clearer directions from the government on what to do and expect. (Duterte later extended the lockdown until April 30 and then again to May 15 for certain areas , including Metro Manila.) Conversations were also dedicated to calls for greater transparency on the breakdown for the P275-billion response fund related to the Bayanihan law. Aside from these topics, the bulk of the 15,000 tweets sampled that centered on Duterte consisted of general reactions to his speech and mostly of people cursing the President and the government, accusing the administration of being “incompetent.” The day’s events on March 30 catalyzed reactions on social media. By April 1, public outrage against Duterte and his administration peaked after he ordered cops and soldiers to “shoot dead” people who broke quarantine protocols. The timing of it could not have been worse. Duterte’s words, delivered during an impromptu televised message on April 1, came hours after the National Bureau of Investigation (NBI) summoned the popular Pasig City Mayor Vico Sotto for a possible violation of the Bayanihan Act, the law which granted Duterte special powers. The NBI did not disclose which specific Pasig policy was under investigation. Sotto had earlier appealed to Malacañang if he could allow tricycles to operate in his city to ferry frontliners and people with emergencies – a pitch that several executive officials rejected. The incident followed with Duterte scolding local government units, warning them to “ stand down ” and abide by orders issued by his office and the government’s coronavirus task force. While the President made no direct mention of Sotto, conversations had related the two incidents to one another. This triggered widespread protests online, with #ProtectVico trending on Twitter (the second time the hashtag trended within two weeks), condemning the government for politicizing response to the crisis. By the time Duterte delivered his April 1 speech, public sentiment against him pushed to a tipping point: #OustDuterteNow trended worldwide on Twitter at 9 pm – the same hour his speech took place – generating almost 500,000 tweets. Analysis by Graphika showed that #OustDuterteNow was a largely organic movement, with little signs of manipulation. Their mapping of the hashtag below shows a wide range of interest groups engaging with the hashtag, with the majority of these segments being largely non-political and clustered instead on entertainment and cultural topics. Among accounts that engaged in discussion critical of Duterte were users from various interest groups like Philippine K-pop, celebrity fan groups, LGBT groups, western pop celebrities, and Philippine culture, celebrities, music. Others that participated were from the Philippine opposition and activists. This suggested a wider online dissatisfaction with Duterte beyond the usual online activists. Atienza said widespread public frustration seen on social media may be because unlike other issues that have hounded Duterte’s administration – such as the drug war or his preference for warmer ties with China – the coronavirus outbreak affects each Filipino. “The pandemic affects everyone, or at least threatens everyone, not just a sector of the population. The threat of the pandemic is so real that there is a feeling of urgency and greater demand for government to act fast and be accountable,” Atienza said. Yet despite this, according to Atienza, Duterte and other government officials have been unable to foster a sense of unity. In response, Filipinos who have increasingly turned to social media during the lockdown took to speaking out against Duterte and his administration. The rather sparse and more loosely connected map (shown below) reflects the traction of #OustDuterte among users grouped by interest on Twitter. The majority of the map showed conversations consisted largely of entertainment and cultural interest segments that lack the density typically observed in politically coordinated accounts. This was evidence that politically focused groups did not appear to be the main organizing force behind the campaign. Ateneo School of Government Dean Ronald Mendoza said public frustration seen in online discussions reflected how the government’s weaknesses were made more obvious during the coronavirus crisis. “Crises test the government’s ability to facilitate collective action (even across its own line agencies) typically exposing the lingering need to boost whole-of-government response capabilities,” Mendoza said. He added, “The government’s seeming insensitivity to the realities of ordinary working citizens who were quarantined, combined with delayed plans to provide income support… all may have also exacerbated the sense that government was insensitive and disconnected from reality.” The sense of frustration and Filipinos’ apprehension over uncertainty brought by the pandemic drowned out any response that attempted to express support for the government’s response. Meanwhile, Graphika’s analysis also showed that about 80% of the accounts that participated in discussion critical of Duterte have more than 100 followers and over 60% of these accounts produced just one tweet using #OustDuterte. The most shared tweets using #OustDuterte also did not originate from influential or celebrity accounts but were posts from seemingly normal users that went viral. About 80% of the accounts that used the hashtag have more than 100 followers and over 60% of accounts produced just one tweet using #OustDuterte. Data showed the #OustDuterteNow trend was largely organic and participatory with little signs of manipulation or coordination. This pointed to a groundswell of negative public sentiments against the President’s handling of the crisis, with users who typically did not discuss politics joining in on these conversations. Signs that propaganda tactics were failing were seen in mid-March when discontent online began to stir. Duterte’s supporters tried several times to resort to old efforts of drowning conversations with praises of the President and mobbing perceived enemies on social media. But these were shut down by angry Filipinos. In fact, at the peak of the online outrage against Duterte, #IStandWithThePresident also trended online, generating more than 130,000 tweets at its height (including tweets that mocked the hashtag). This, however, was largely drowned out by #OustDuterteNow. Another attempt to push out messages against those critical of the administration also contributed to the build up of public frustration by April. On March 18, administration officials and supporters blasted Sotto for allowing tricycle drivers to operate while Luzon was on lockdown. This included blogger-propagandist Mocha Uson who called Sotto “ pabebe ” (childish) on her Facebook page. Uson’s page has a following of some 5 million users. This was in keeping with the type of systematic and sustained response seen in the past 3 years against journalists and critics of the President: officials around Duterte hit perceived critics on the ground, while online supporters pounded them en masse. This time around, however, this attempt was not met with the usual silence. #ProtectVico quickly trended online, generating over 37,000 tweets from almost 22,900 users. It then snowballed into an online campaign targeting Mocha Uson, with users encouraging everyone to report her blog on Facebook in an attempt to close it down. On March 20, her Facebook page became unavailable . People speculated that she might have deactivated the page herself. In celebration, #MochaUsonIsOverParty trended on Twitter, with 24,000 tweets from over 11,800 distinct accounts. Campaigners then started targeting other blogs notorious for spreading pro-Duterte propaganda, such as Crabbler, Mark Lopez, and Mr Riyoh. Like #OustDuterteNow, the data suggests that #ProtectVico and #MochaUsonIsOverParty was largely organic with little signs of manipulation. Over 80% of the accounts have between 100-1,000 followers and over 65% of accounts produced just one tweet using either (or possibly both) combination of hashtags. This laid the groundwork for widespread dissatisfaction seen online on April 1. The most retweeted tweets to feature either hashtag were in support of Sotto’s actions to control the COVID-19 outbreak or were used to counter criticism from blogger Mocha Uson. Some users went as far as requesting social media administrators to suspend her accounts. These posts were popular across all groups including both the culture and entertainment segments critical of Duterte – the same ones that participated in the bulk of conversations on April 1. Later on April 10, Twitter “hundreds of accounts” tweeting under specific hashtags meant to defend the Philippine government response to the coronavirus pandemic. An email from Twitter to The Washington Post , said the accounts in question violated Twitter’s policies against platform manipulation and spamming. This includes posting duplicate content across multiple accounts, making duplicate or multiple accounts, and sending a large number of unsolicited replies or mentions. The Washington Post  report noted that hashtags in support of Duterte followed after public outcry over government actions against the poor during the coronavirus quarantine. These hashtags included #IStandWithThePresident and #YesToABSCBNShutdown. The mass takedown by Twitter was part of a wider effort of other social media platforms to get rid of accounts that spread disinformation during the pandemic. It’s also the first announced case of Twitter actually taking down a network connected to the propaganda machine. When it came to the Duterte administration’s handling of the outbreak – genuine online users drowned out propaganda tactics. As the coronavirus pandemic rages, political analysts say the outbreak may be Duterte’s biggest test yet. Now more than ever, Filipinos are demanding transparency and accountability in government’s response. The stakes are high as missteps in government’s response could mean the loss of lives due to the disease. For Mendoza, the crisis carries a high political cost for Duterte as the outbreak hits several of his main constituencies in both the middle class and overseas Filipino workers. “If government is unable to respond effectively to mitigate the crisis impact, then we may witness change in political support,” he said. According to Atienza, Duterte and his team may have touted the war on drugs, massive infrastructure programs, and development in regions outside Metro Manila as legacies of his administration, but what is clear is the pandemic “has changed the agenda for the rest of his term.” “President Duterte’s leadership style appears not fit for this crisis. This is a different kind of crisis that requires reliance on experts and stakeholders as well as making sure people are involved and not left behind,” she added. “Whether he likes it or not, he will now be judged based on what he and his administration had done and did not do during the pandemic,” Atienza said. – Rappler.com How does this make you feel? </t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Networked propaganda,Rodrigo Duterte</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Government offensive: Info operations attack media to manage SEA Games PR crisis</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>https://www.rappler.com/newsbreak/investigative/246186-government-offensive-info-operations-attack-media-manage-pr-crisis-sea-games-2019/</t>
+        </is>
+      </c>
+      <c r="D23" s="2" t="n">
+        <v>43801.58028935185</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">From #Seagames2019fail to #Seagamesnotafailure – Rappler maps how the conversations on the SEA Games pan out on social media By Don Kevin Hapal  Published 9:55 PM, December 02, 2019 </t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Networked propaganda: False narratives from the Marcos arsenal</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>https://www.rappler.com/newsbreak/investigative/245540-networked-propaganda-false-narratives-from-the-marcos-arsenal/</t>
+        </is>
+      </c>
+      <c r="D24" s="2" t="n">
+        <v>43791.46261574074</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Conclusion: For the Marcos comeback playbook, facts don't matter  READ: Part 1 | Networked Propaganda: How the Marcoses are using social media to reclaim Malacañang    READ: Part 2 | Networked Propaganda: How the Marcoses are rewriting history    MANILA, Philippines – “Perception is real, the truth is not.” Imelda Marcos said this in a recently released documentary, The Kingmaker . This seems to be the ethos of the Marcos comeback playbook. Beyond justifying the family’s wealth and denying massive corruption during the Martial Law period, the Marcos propaganda network focused its energies on hyping up “achievements” of the Martial Law regime, denying abuses, and vilifying rivals. The facts don't matter. “Achievements” were either exaggerated or manufactured. That these were not previously reported on were explained as being the fault of “biased” media, which supposedly kept the information “hidden” from the public.  Exaggerated achievements  Much of the content touting the supposed “achievements” of the Ferdinand Marcos presidency were copied and reposted over and over like chainmail. The lists typically included a litany of infrastructure projects that the Marcoses built. Such lists included a combination of true and many false and misleading claims. For instance, it's not true that Marcos built the first airport in Asia. Further, Ninoy Aquino International Airport, the country’s main airport and formerly known as the Manila International Airport, had already existed before Marcos took office.    Often reiterated and rehashed was the claim that the Philippines was the "richest country in Asia" during the Marcos years. It never was. The peso-dollar exchange rate during that time supposedly stood at P1.50-P2 to the dollar . This is not true. Official data from the Bangko Sentral ng Pilipinas (BSP) showed the Philippine peso was already valued at P3.91 per dollar when Marcos came into power in 1965. By the time he was ousted in 1986, one dollar was equivalent to P20.46 – depreciating by 423.46%.  Even foreign-funded programs were touted as Marcos achievements. These included supplemental feeding programs such as the nutribun and bulgur for students in public elementary schools. Bulgur grains and the ingredients for nutribun were actually supplied by the United States Agency for International Development (USAID) as part of its Food for Peace Program.  False dichotomy  Reviving the Marcos name came at the expense of the family’s nemesis, the family of the late senator Benigno "Ninoy" Aquino Jr and the press. In a bid to proclaim Marcos as the “best president” the Philippines ever had, weaponized memes framed the narrative as a Marcos vs Aquino play. Some went as far as claiming that the “dilawans” have been in power for the past 30 years.      This is misleading at best. When the Marcos dictatorship fell in 1986 due to the EDSA People Power revolt, Aquino’s widow, Corazon “Cory” Cojuangco Aquino assumed the presidency. Fast forward to 2016, another Aquino was the outgoing president – Benigno Simeon Aquino III, the only son of Ninoy and Cory. Three presidents served in office in between the tenure of the two Aquinos: Fidel Ramos, Joseph Estrada, and Gloria Macapagal Arroyo. Of all the post-EDSA presidents, the longest serving was Arroyo, who assumed part of the remaining term of Estrada after the latter was ousted in 2001, and got elected for another 6 years. Memetic propaganda essentially erased or disregarded achievements and economic growth that happened during the tenure not just by the Aquinos, but of all post-EDSA presidents combined. Ironically, all the 3 other presidents – Ramos, Estrada and Arroyo – supported the bid of Rodrigo Duterte for the presidency in 2016.  'Hidden' history  “Hidden history” and the “biased” press, according to the narrative, were also to blame for unknown or “unreported” sins of the Aquino family. One of the charges leveled against the Aquinos pertained to Hacienda Luisita, which was exempted from the Comprehensive Agrarian Reform Program enacted during Cory Aquino’s term. While this claim is rooted in real events, the way it is presented is misleading. The Hacienda Luisita case got a lot coverage from mainstream media. One claim that was widely circulated by one of the pro-Marcos Duterte propagandists was that the Central Intelligence Agency (CIA) of the United States supposedly "revealed" recently that Cory Aquino requested the US for airstrikes against Filipinos in 1989. This was misleading. While Cory did ask for US air support during the 1989 coup d’etat, these requests were not hidden or "recently revealed." They were headlined in major local and international publications at the time.       Some of these claims bordered on the ridiculous. A popular claim that Rappler spotted more than once was that Ninoy Aquino was a naturalized Malaysian citizen and that he was carrying both a Filipino and a Malaysian passport when he died. There is no proof that this ever happened. Malaysia was officially recognized as a sovereign country only in 1957. The naturalization law of Malaysia also requires an individual born outside Malaysia to have resided in the country for at least 10 years to acquire citizenship. Aquino, who was born in 1932, would have had to fulfill this requirement to gain citizenship. Another claim that went viral said that Cory wore Imelda Marcos’ necklace , which has allegedly been missing from the collection of the Presidential Commission on Good Government. Others said Kris Aquino, and even former chief justice Maria Lourdes Sereno wore the necklace. None of these were true. Nevertheless, these claims got thousands of shares on social media.  Lying about Martial law abuses  This is not to say that all the false narratives about the late dictator or the Martial Law era came from the Marcoses themselves. They persisted, some historians said, because the family never publicly denied them. In fact, the Marcoses also made their own false claims about the period.   MARTIAL LAW. Ex-senator Bongbong Marcos interviews ex-defense minister and Senate president Juan Ponce Enrile. Screenshots from Bongbong's YouTube account  On September 20 and 21, 2018, the 46th anniversary of the declaration of Martial Law, Bongbong sat down with former Marcos defense minister Juan Ponce Enrile to talk about his father's 20-year rule. Rappler debunked 3 of Enrile’s false claims from their conversation: that the Marcos government only executed one person, that there were no massacres, and that the Jabidah massacre was a mere invention. (READ: LIST: False claims of Juan Ponce Enrile on Martial Law ) In a radio interview in January, Imee Marcos claimed that she was a minor during the Martial Law period. As such, she said, she could not admit guilt over the events that happened during that time. Again, this was a lie. Imee was about to turn 17 when her father declared Martial Law, which means she was no longer a minor for 13 out of 14 years of Martial Law. The list of lies and misleading claims continue to this day. And for the Marcoses, the playbook appears to be working. In May 2019, despite being exposed by most of mainstream media for lying about her academic achievements, Imee Marcos won a seat in the Philippine Senate. – with Vernise Tantuco /Rappler.com  </t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Networked Propaganda: How the Marcoses are rewriting history</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>https://www.rappler.com/newsbreak/investigative/245402-networked-propaganda-marcoses-rewriting-history/</t>
+        </is>
+      </c>
+      <c r="D25" s="2" t="n">
+        <v>43790.53876157408</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Part 2: Messages posted on groups and pages monitored by Rappler's Sharktank typically also glorified the virtues of authoritarian rule  READ: Part 1 | Networked Propaganda: How the Marcoses are using social media to reclaim Malacañang    MANILA, Philippines – From the time Rappler started ramping up its fact-checking efforts, it has spotted hundreds of dubious claims related to the Marcoses and Martial Law on social media. Claims ranged from those that attempted to explain away the Marcos wealth – to those that “exposed” the sins of their nemesis: the family of the late Senator Benigno “Ninoy” Aquino Jr, whose assassination triggered the dictator’s downfall. Apart from attempting to erase the history of abuse and corruption by the Marcoses during the Martial Law years, the claims have  recurring themes. What is often described as "shocking" information is generally portrayed as having been “hidden” from the public by historians and the “biased” press. Messages posted in groups and pages monitored by Rappler's Sharktank typically glorified the virtues of authoritarian rule. To a significant extent, the campaign focused on disputing or revising historical accounts about the Marcoses' ill-gotten wealth. The table below lists pages and groups where dubious claims tracked and fact checked by Rappler's fact check team have been shared. All together, these content generated over a million shares, reactions, and comments on Facebook.       Denying Marcos kleptocracy  One example of this is a claim posted in May 2014, ahead of the 2016 elections, by popular Facebook page Pinoy Rap Radio, which also tried to dispute the truth about the Marcos wealth. If Ferdinand Marcos stole billions from Filipinos, one of the page’s posts argued, why was it that succeeding presidents after him “can not show any proof at all?” The author also claimed that Imelda Marcos, the widow of the dictator, “won every corruption case” that was hurled at her.   Both claims were lies even as authorities have been reluctant to arrest Imelda . In a 2003 ruling, the Philippine Supreme Court forfeited seized Marcos assets after finding that Ferdinand and Imelda Marcos failed to justify the acquisition of their assets which exceeded their salaries as public officials. (For updates on the Marcos cases, read: What's the latest on cases vs Imelda Marcos, family? ) The truth did not stop the post from getting widely circulated on Facebook – it got more than 331,000 shares, more than 38,000 comments, and more than 369,000 reactions before it was finally spotted and fact checked by Rappler on November 15, 2018. Pinoy Rap Radio was not the only viral content page involved. Months after Pinoy Rap Radio’s post denying Marcos’ guilt, various accounts and pages on Facebook reposted the claim. Pages that iterate this same message include Blessed Be Philippines, Team Marcos-The Universal Movement, The Pandora's Box, and Batang Marcos, among others.        Created on October 25, 2016 and among the pages that have repeatedly posted false claims about the Marcos wealth, Batang Marcos is managed by 4 administrators based in Macau, according to its page transparency tab. Among dubious content it posted was a claim about the Tallano royal family of the Maharlika kingdom that supposedly encompassed the entire Philippine archipelago and neighboring countries during the pre-colonial era. The tons of gold allegedly owned by the Marcoses – ranging from fantastic claims of hundreds of thousands of tons to a million tons – were supposedly given by the Tallano family to the Marcoses. This claim is reiterated by Bible-quoting social media influencer Sangkay Janjan, who has posted a number of videos exagerating Marcos achievements and justifying their wealth on his Facebook page and YouTube channel. In one video, Sangkay Janjan even flashes a map of the alleged Maharlika kingdom.    These are all false claims. There is no proof that such a kingdom ever existed , according to historians. Nor is there proof that a royal family named Tallano ever ruled over this kingdom. Even Tadhana: The History of the Filipino , the series of history books that Marcos bylined to herald his New Society, never mentioned Maharlika.  Millions reached, no denials  Altogether, these false claims have logged millions of impressions on Facebook and YouTube. One of the Batang Marcos posts about Maharlika and the Tallanos got as many as 80,000 shares before it got fact checked by Rappler. Sangkay Janjan’s YouTube video with the Maharlika kingdom map has been viewed over a million times. Videos on YouTube that claim the Marcoses own a million tons of gold and that this gold will “save the world” have also gotten over 1 million views as of writing. The number of followers of Facebook pages, groups, influencer accounts, and YouTube channels involved in this massive propaganda effort amount to millions. The people behind these channels appear impervious to fact checks. Pinoy Rap Radio did not respond to Rappler’s requests for an explanation about how they came to their conclusion. After Rappler published its fact check on the Pinoy Rap Radio claim denying Marcos corruption, the page administrators merely deleted the post without issuing corrections. They also deleted similar content posted on their page. Rappler sought to interview Sangkay Janjan about the content he has been posting but he did not agree to an interview. Instead of issuing a correction in relation to a fact check done by Rappler , he defiantly posted a live video further exaggerating Marcos achievements. It does not help that the Marcoses never denied nor commented on these claims. They have not granted Rappler’s request for an interview regarding these false claims and the activities of their campaign team on social media. Imelda herself fanned this myth because she has been featured in interviews talking about the amount of gold her family supposedly owns . The Marcoses and President Duterte have also been saying that the Marcos family intends to give away their wealth without acknowledging the corruption charges.  Vulnerable spot  There could be a method to this madness. Reports about the Marcos wealth obtained illegally or through corruption have been a politically vulnerable spot for the family. Imelda Marcos was convicted of 7 counts of graft in November 2018. In 2003, the Philippine Supreme Court rendered final judgment forfeiting in favor of the Philippine government funds that were recovered from the Marcoses’ Swiss deposits amounting to US$658,175,373.60 as of January 31, 2002.   POST-CONVICTION FREEDOM. File photo of former First Lady and Ilocos Norte Representative Imelda Marcos during a November 16, 2018, hearing at the Sandiganbayan, which granted her bail despite conviction of 7 counts of graft. Photo by Jire Carreon/Rappler The government's petition for forfeiture was granted by the High Court on grounds that the total amount of the Swiss deposits was "considerably out of proportion to the known lawful income of the Marcoses ." Thus, disputing these or revising historical accounts about the Marcos wealth have been integral to the Marcos strategy of strengthening, if not consolidating, political dominance. And it seems that the strategy is working. Two years after the Marcos propaganda campaign ramped up on social media , Bongbong Marcos almost won the vice-presidential race in a very narrow contest. The results are still being contested. (To be concluded) –  with Vernise Tantuco/ Rappler.com     READ: Conclusion | Networked propaganda: False narratives from the Marcos arsenal       Editor's Note:   As a matter of policy, Rappler does not hyperlink to channels and content proven to have been false or which have been used to spread disinformation or misinformation to avoid amplifying these false claims.  </t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Networked propaganda: How the Marcoses are using social media to reclaim Malacañang</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>https://www.rappler.com/newsbreak/investigative/245290-marcos-networked-propaganda-social-media/</t>
+        </is>
+      </c>
+      <c r="D26" s="2" t="n">
+        <v>43789.55070601852</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Disinformation, coordinated amplification, use of an extensive network of anonymously-managed pages and groups are part of the Marcos comeback playbook MANILA, Philippines – Massive amounts of propaganda and targeted disinformation produced and amplified by an extensive network of websites, Facebook pages and groups, YouTube channels, and social media influencers appear to be part of a systematic campaign to burnish the image of the Marcoses and pave the way for their further rise in Philippine politics. The content that this network circulated included numerous claims that sought to alter public perception of the Marcoses by either downplaying or outrightly denying kleptocracy and human rights violations during the Martial Law years, exaggerating Marcos achievements, and vilifying critics, rivals, and mainstream media. Many of these claims have since been debunked and proven to be false. A number of pages and accounts that are part of this network have also been taken down by Facebook for posting "spammy content" and  "coordinated inauthentic behavior." The campaign ramped up two years ahead of the 2016 elections and continues to produce and amplify content on a scale that rivals the volume of content circulated by mainstream media groups to date. It involves a network of Marcos and Duterte fan pages and groups, meme and viral content pages, pages circulating claims of allegedly “hidden facts” in Philippine history, and pages attacking and undermining mainstream media. Personal accounts and pages managed by key social media influencers known for staunchly defending President Duterte and his administration’s policies also took part in the campaign. The pages and groups involved were observed to be systematically sharing and amplifying each other’s content, along with content from known pro-Duterte and pro-Marcos social media influencers. Made with Flourish  Fan pages &amp; groups  The campaign ramp up included the creation of hundreds of fan groups and pages supporting the Marcos family. As of September 5, 2019, the Sharktank, a Rappler database, has tracked over 360 pages and over 280 groups supporting the family – whether it’s now-senator Imee Marcos, Ferdinand “Bongbong” Marcos Jr, their late father, or family matriarch Imelda Marcos. (The Sharktank is a Rappler database built to monitor Philippine conversation channels within Facebook – through public pages, public groups, and publicly available posts.) The graph below shows the dates the pages were activated based on the first post from these pages that the Sharktank spotted. Made with Flourish On the other hand, the graph below shows the dates when groups were activated based on the first post from these pages that the Sharktank spotted. Made with Flourish The only other local politicians who rival the Marcoses in terms of number of fan groups and pages are President Duterte himself, and Senator Bong Go. Rappler has tracked around 1,800 Duterte fan pages and hundreds of fan groups to date. Initial Duterte fan pages were created as part of the ramp up for the 2016 presidential elections. Most, however, were created after Duterte assumed office. Rappler has also detected similar messaging in relation to Martial Law and the Marcos dictatorship across pro-Duterte and pro-Marcos pages. As the graph shows, while a few Marcos pages were created much earlier, the creation of new pages per month really started to ramp up in 2014, around the time former first lady Imelda Marcos first mentioned she wanted her son to run for president. It was in July 2014, during her 85th birthday celebration , that Imelda Marcos hinted at a plan for a Marcos return to Malacañang. She said her son Bongbong, who was already senator at the time, was “qualified” to contest the presidency in 2016. The graph above also indicates that new fan pages were created even after the 2016 elections. Further ramp up happened ahead of the 2019 elections when another Marcos offspring, Imee Marcos, ran for the Philippine Senate.  Reclaim Malacañang  Imelda, in 2014, said she still has a “vision” to help the Filipino people and that returning to Malacanang would be a great help in implementing her projects.   POWER BID. Vice presidential candidate Bongbong Marcos joins Ilocos Norte 2nd District Representative Imelda Marcos and Ilocos Norte Governor Imee Marcos after they file their certificates of candidacy for local elective positions during the 2016 elections. Photo from the Provincial Government of Ilocos Norte But this was not the first time that the Marcoses attempted a return to Malacañang. Since they were evicted in 1986, Imelda herself attempted to return to the Palace twice. The first attempt was in 1992, when she ran for president under her husband’s Kilusang Bagong Lipunan party. She lost the race , tying at 5th place with then-Senate president Jovito Salonga, getting 10% of the votes. The second time was supposed to be in 1998, but she withdrew days before the elections . She did not have a chance to win anyway at the time. Already convicted of two counts of graft by then, an exit poll of Social Weather Stations ranked her 9th out of 11 candidates , with only 0.9% saying they would vote for her.  (The Supreme Court voided her conviction months after the polls. For more on the Marcos cases, READ: What's the latest on cases vs Imelda Marcos, family? ) Between 1986 to 2009, no Marcos made it to national office. Bongbong Marcos himself also attempted to bag a national post in 1995 when he ran for senator under the Kilusang Bagong Lipunan party founded by his father and as part of the Nationalist People's Coalition ticket. He finished the race ranking a miserable 16th place with more than 8 million votes. From that point, it took more than a decade before a Marcos sought national office again. It was not until 2010 when Bongbong finally won a Senate seat. He ranked 7th place , with 13,169,634 votes. Winning the Senate is one thing. The question was whether a Marcos was ready for the final goal: getting Malacañang back. It was doubly difficult because in the 2010 elections, the son of Marcos nemesis, Benigno "Ninoy" Aquino Jr, Benigno Simeon “Noynoy” Aquino III, won as president on an anti-corruption platform. Social media was a handy trick in the bag. (To be continued) – with Vernise Tantuco and Akira Medina/ Rappler.com      READ: Part 2 | Networked Propaganda: How the Marcoses are rewriting history  READ: Conclusion | Networked propaganda: False narratives from the Marcos arsenal     </t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Tip of the iceberg: Tracing the network of spammy pages in Facebook takedown</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>https://www.rappler.com/newsbreak/investigative/215256-tracing-spammy-pages-network-facebook-takedown/</t>
+        </is>
+      </c>
+      <c r="D27" s="2" t="n">
+        <v>43400.5</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Many of the pages in these networks have shared false or misleading articles By Rappler Research Team  Published 8:00 PM, October 27, 2018 </t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Isaiah Thomas out for rest of playoffs</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>https://www.rappler.com/sports/nba/170476-boston-celtics-isaiah-thomas-playoffs-hip-injury/</t>
+        </is>
+      </c>
+      <c r="D28" s="2" t="n">
+        <v>42876.11682870371</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SUMMARY This is AI generated summarization, which may have errors. For context, always refer to the full article. AFP BOSTON, USA – Boston Celtics guard Isaiah Thomas will be sidelined for the rest of the postseason after aggravating a hip injury during game two of the Eastern Conference finals, the NBA team announced on Saturday, May 20. The 28-year-old Thomas initially injured his hip in a game against the Minnesota Timberwolves on March 15, and then aggravated it during game 6 of the second round series against the Washington Wizards. “Isaiah has worked tirelessly to manage this injury since it first occurred,” said Celtics team doctor Brian McKeon. “The swelling increased during the first two games against Cleveland, and in order to avoid more significant long-term damage to his hip, we could no longer allow him to continue.” Thomas has been diagnosed with a femoral-acetabular impingement which affects the ball joint in the hip socket. Thomas did not travel with the team to Cleveland for game 3 on Sunday. The Cavaliers lead the series, 2-0. – Rappler.com How does this make you feel? </t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Disinformation,Networked propaganda</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>[ANALYSIS] Viber: The next frontier for political propaganda in the Philippines?</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>https://www.rappler.com/voices/thought-leaders/analysis-viber-next-frontier-political-propaganda-philippines/</t>
+        </is>
+      </c>
+      <c r="D29" s="2" t="n">
+        <v>44549.49818287037</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SUMMARY This is AI generated summarization, which may have errors. For context, always refer to the full article. As is well-known, Facebook is widely used across Southeast Asia, especially in the Philippines, where 99% of internet users have Facebook accounts and 98% use Facebook Messenger , mostly to communicate with family and friends. In comparison, the use of the messaging app Viber is very low – only 5% of internet users use it. However, Viber use is rapidly growing in the Philippines and with it, its political significance grows, too. The Propaganda Lab at the Center for Media Engagement at UT Austin conducted 21 interviews in the Philippines, Indonesia, Myanmar, and Ukraine , and found that Viber is being used for the spread of political propaganda in the Philippines in particular . While Facebook remains widely used for propaganda in Indonesia, for instance, our interviewees in the Philippines articulated that Viber has been “invaded” by Duterte’s government. So, will Viber be the next hotbed of disinformation or misinformation exploited by an authoritarian leader? Disinformation and political propaganda are rampant on Facebook across Southeast Asia but similar phenomena on encrypted messaging applications (EMAs) are underexplored. Apps that use end-to-end encryption (E2E), which tout that only the sender and receiver can see what messages say, are growingly popular across the globe . Troublingly, they are increasingly becoming spaces for mis- and disinformation just like “traditional” social media. They have even led violence to erupt in the offline world, such as mob lynchings in India after disinformation spread on WhatsApp , and played a role in anti-democratic movements, such as the Capitol riot in the United States . The emerging use of Viber, an app that offers E2E in 1-on-1 and group chats (though not in channels or communities) , looks like the next frontier for political propaganda and disinformation in the Philippines and Southeast Asia writ large. For instance, representatives from the Presidential Communications Operations Office interviewed by us explained that the government established Viber groups that include over two million users to distribute information from the government to Filipinos. In addition to government announcements, these groups serve as an avenue to encourage support for President Duterte on a platform that is sure to reach a widespread audience. According to two representatives from the communications office, their goal is to make the president visible – even “ubiquitous.” They aim to make content as entertaining as possible, tailored specifically to younger audiences. One example is sticker campaigns. Graphic designers in the communications department have designed sticker packs with President Duterte’s image paired with politically motivated phrases – people in his office would call this increasing support, but a cybersecurity strategist we spoke to (who is also a former politician), called these “Duterte ads.” He considered these strategies to be more than just spreading presidential news – he explicitly called it “propaganda.” In addition to calculated strategies like sticker packs, government officials thoughtfully select which platforms to engage on as well. “We use Facebook Messenger to blast information to the public.” Although they “try to blast it on all platforms,” they particularly aim to target young folks (millennials and younger) through emerging platforms like TikTok and Viber. This is strategic – the number of TikTok users in the Philippines is increasing , just like Viber. “Filipinos want to go to social media as an escape,” one of the officials told us, “so you must package your content in the most entertaining and trendiest way possible to relate, especially to the millennials.” Their strategies are deliberately coordinated in order to reach the most emerging users. The representatives we spoke to were adamant that such content was not pushed by trolls. “For us, social media is just an additional task of our public information officers.” In fact, a main part of their job description includes content creation and social media management. The creation of in-house social media teams signals how vital social media has become for the Duterte regime. “We don’t hire external outfits or groups to run our social media,” they told us. However, while the people we spoke with who work in Duterte’s communications office would (and did) vehemently deny the use of troll farms, it has been exposed in investigative reporting and academic work alike . The use of Viber differs greatly across different cultures and countries. In Myanmar, for instance, it’s not widely used, and in Indonesia WhatsApp reigns. In general, EMAs are often used to connect individuals into small groups from families to community social groups; with the unintended side effect, however that – “lots of disinformation spreads between family and friends,” as a cybersecurity strategist told us. Hence the additional question arises if Viber will not only be the next outlet for disinformation in the Philippines but also co-opted by troll farms. One man we spoke to in Indonesia (we would refer to him as a troll, but they call themselves “buzzers”) told us about his strategies for political propaganda on traditional social media like Facebook and YouTube: he and his team each run 50 or more accounts, orchestrating fake arguments between the accounts about political candidates. Ultimately, all of the “people” (fake accounts) concede and support the candidate the buzzer/troll was hired to increase support for. This strategy, he told us, is not possible on EMAs. However, he and other interviewees explained that by pushing out positive information about one candidate and negative disinformation about the other, they can still affect public opinion and likely, elections. Ultimately our research has discovered that EMAs are falling prey to exploitation just as other social media sites have. However, there is another side to this challenge, namely the receptiveness and potential engagements of EMA users to disinformation and propaganda. In the Philippines in particular, citizens have been trying to push back against an authoritarian leader – so while online spaces such as Viber and TikTok present opportunities for state actors to manipulate young folks, who are allegedly especially at risk for believing fake news , this research also wants to highlight the opportunities for pushback. For example, EMAs are useful to communicate in private and mock government propaganda or engage in fact-checking to expose government propaganda. For this, researchers must keep a finger on the pulse of disinformation campaigns on emerging platforms since actors, such as the Filipino government, adapt to the ever-changing social media trends for their own goals. – Rappler.com Katlyn Glover is a researcher and graduate student at the Propaganda Lab at the Center for Media Engagement at the University of Texas at Austin, where she researches disinformation and political propaganda on emerging technologies. Zelly Martin Geurink is a researcher and PhD student at the Propaganda Lab at the Center for Media Engagement at the University of Texas at Austin, where she researches disinformation and political propaganda, especially as they pertain to women. How does this make you feel? </t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Disinformation,mobile phone technologies,social media platforms</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Bulls to retire Derrick Rose's No. 1 jersey</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>https://www.rappler.com/sports/nba/chicago-bulls-retire-derrick-rose-jersey/</t>
+        </is>
+      </c>
+      <c r="D30" s="2" t="n">
+        <v>45891.39377314815</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SUMMARY This is AI generated summarization, which may have errors. For context, always refer to the full article. CHICAGOu2019S OWN. Derrick Rose played at the peak of his powers with the Chicago Bulls. NBA.COM The Chicago Bulls will retire former NBA MVP Derrick Rose’s No. 1 jersey on January 24, the team announced Thursday, August 21. The Bulls will host the Boston Celtics that night at the United Center. Rose, 36, announced his retirement from the league over social media last September. The No. 1 jersey has not been worn by a Bulls player since Rose was traded to the New York Knicks in 2016. Michael Carter-Williams and Anthony Morrow were issued the number but switched after fan backlash. Rose will be the fifth player in Bulls history to have his number retired, joining Jerry Sloan (No. 4), Bob Love (10), Michael Jordan (23), and Scottie Pippen (33). Rose was selected by his hometown Bulls with the top overall pick in the 2008 NBA Draft and was named the 2008-09 Rookie of the Year. At 22, Rose became the youngest player in league history to be named the NBA MVP during the 2010-11 season. Chicago was 245-161 (.603) in games in which Rose played. In his MVP season, he led the Bulls to their first Eastern Conference Finals appearance since 1998 — the final season of the Bulls’ second NBA championship three-peat. Rose’s career took a turn for the worse after he tore an ACL during the first round of the 2012 playoffs. He sat out the following season and was limited to 10 games in 2013-14. A three-time All-Star, Rose posted career averages of 17.4 points, 5.2 assists, and 3.2 rebounds in 723 career games (518 starts) with the Bulls, Knicks, Cleveland Cavaliers, Minnesota Timberwolves, Detroit Pistons, and Memphis Grizzlies. Injuries limited Rose to 24 games (seven starts) with the Grizzlies in 2023-24 as he averaged 8.0 points, 3.3 assists, and 1.9 rebounds. – Rappler.com How does this make you feel? </t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Chicago Bulls</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Adidas visits Indigenous Mexican town to apologize for sandal design</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>https://www.rappler.com/life-and-style/style/adidas-visits-indigenous-mexican-town-apology-sandal-design/</t>
+        </is>
+      </c>
+      <c r="D31" s="2" t="n">
+        <v>45891.38153935185</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SUMMARY This is AI generated summarization, which may have errors. For context, always refer to the full article. Traditional Indigenous sandal are pictured in a workshop as Juan Aquino makes a sandal in Villa Hidalgo Yalalag while the Mexican government stepped in on Friday to mediate a dispute between Indigenous artisans from Oaxaca and Adidas over cultural appropriation claims involving the "Oaxaca Slip On" shoe, designed by Willy Chavarria, in Villa Hidalgo Yalalag, Oaxaca, Mexico, August 9, 2025. REUTERS/Jorge Luis Plata VILLA HIDALGO YALALAG, Mexico — Adidas ADSGn.DE executives visited a small Indigenous town in the mountains of southern Mexico on Thursday to offer an apology over a sandal-inspired shoe design that Mexico’s government had blasted as cultural appropriation. The German sportswear company sent representatives from its Mexican unit to Villa Hidalgo Yalalag, a town in Oaxaca state, to deliver the comments in person after issuing a written apology last week. The issue related to the “Oaxaca Slip On,” designed by Mexican-American designer Willy Chavarria, which locals say closely resembles their traditional handmade huarache sandals. “We understand this situation may have caused discomfort, and for that reason, we offer a public apology,” Karen Gonzalez, head of Legal and Compliance at Adidas Mexico, told a few dozen people gathered at an outdoor sports field. The event included traditional music and attendees in Indigenous attire. Gonzalez said Adidas would in future seek collaboration with Villa Hidalgo Yalalag to ensure respect for its cultural heritage. The community is home to fewer than 2,000 people. “Thank you very much for keeping your word,” said Mayor Eric Fabian. “(Our cultural heritage) is something we safeguard very carefully. Yalalag lives from its crafts,” he added. The controversy drew national attention earlier this month when Mexican President Claudia Sheinbaum criticized Adidas and announced plans to explore legal avenues to protect Indigenous communities from alleged cultural appropriation by big companies. Mexico has previously accused other big-name global fashion players of exploiting Indigenous designs without consent. – Rappler.com How does this make you feel? </t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>fashion brands,fashion industry,Mexico,sports brands</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Kathryn Bernardo returns to TV with Dreamscape Entertainment after 15 years</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>https://www.rappler.com/entertainment/celebrities/kathryn-bernardo-tv-comeback-dreamscape-entertainment/</t>
+        </is>
+      </c>
+      <c r="D32" s="2" t="n">
+        <v>45891.37671296296</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SUMMARY This is AI generated summarization, which may have errors. For context, always refer to the full article. RETURN. Kathryn Bernardo is heading back to TV with Dreamscape Entertainment. ABS-CBN MANILA, Philippines – Asia’s Superstar is returning to the small screen! Kathryn Bernardo will be returning to ABS-CBN primetime television, reuniting with Dreamscape Entertainment after 15 years. ABS-CBN officially announced her comeback on Friday, August 22. “The wait is over. SHE IS BACK AND READY. The Asia’s Superstar, Kathryn Bernardo, is now ready for her grandest comeback,” Dreamscape wrote on YouTube. This marks the Filipina actress’ first TV project with Dreamscape in 15 years, after she starred in her breakout role as Mara David in the 2010 hit drama Mara Clara , where she starred alongside Julia Montes, who played her rival Clara del Valle. The series was a remake of the 1992 classic. Details about the new series are still under wraps, such as the cast, storyline, or production timeline. The 30-second video teaser of Bernardo’s comeback was released on social media, showing Bernardo in a glam shoot. Her most recent television role was in the 2022 romantic comedy 2 Good 2 Be True , with former love team partner Daniel Padilla. On the big screen, Bernardo headlined The Hows of Us (2018), Hello, Love, Goodbye (2019), and its 2024 sequel Hello, Love, Again , now the highest-grossing Filipino film of all time. She also starred in A Very Good Girl (2023) with Dolly de Leon and previously appeared in films like Barcelona: A Love Untold (2016). She is also a judge in Pilipinas Got Talent . Dreamscape Entertainment, ABS-CBN’s drama production unit, is known for popular teleseryes, such as including FPJ’s Ang Probinsyano, Batang Quiapo, Lavender Fields, Dirty Linen, Senior High, and more. – Rappler.com How does this make you feel? </t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>ABS-CBN,Filipino celebrities,Tv Shows</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>[Pastilan] Floods come, budgets swell</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>https://www.rappler.com/voices/thought-leaders/pastilan-floods-come-budgets-swell/</t>
+        </is>
+      </c>
+      <c r="D33" s="2" t="n">
+        <v>45891.36858796296</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SUMMARY This is AI generated summarization, which may have errors. For context, always refer to the full article. Sam Calleja/Rappler Candating, a riverside barangay in Pampanga’s 4th District, might look as though it has been singled out for some cruel fate. The people of that village in Arayat probably know the cycle by now: floodwater in their homes, mud in their lives. But what they should not have to endure is the further indignity of watching their plight converted into a feeding trough for corrupt people in government and their favored contractors. Senator Ping Lacson , consulting what might be called the ledgers of farce, laid out the numbers before the Senate. In 2018, he said, a slope protection in Candating was built for P20 million. Five years later, its repairs — not new construction, just repairs – cost P91 million. By 2024, the cost had swollen further to P183 million, as if this public works farce, when diced into smaller servings, could be mistaken for respectability. And then, Lacson added, another P100 million was waiting in the wings, halted only by Malacañang’s late intervention. One is tempted to ask: Do we call this “infrastructure”? No, this looks like an open-air theater of decay, staged with concrete props on a riverbank stage. The pattern is pitiless. The floods come, the walls crumble, and the budgets swell. One collapses, the other cashes in. And the same contractor, identified by Lacson as Eddmari Construction and Trading, keeps bagging the contracts. It seems Eddmari Construction has been everywhere, and not merely within the confines of the Department of Public Works and Highways (DPWH). The Pampanga-based firm has acquired a national footprint, appearing wherever there is ruin to be rebuilt or funds to be disbursed. Its record is hardly spotless: once delisted as an accredited government builder , it had six projects terminated by the National Housing Authority in 2018. That was, for all intents and purposes, an institutional rebuke not easily earned, though apparently just as easily forgotten. Yet Eddmari’s case shows that blacklisting in this country is more like a pause button than a stop sign. In 2019, or a year later, the Duterte administration awarded it with a P2.2-billion contract to demolish damaged structure and clear debris in war-torn Marawi City , through a “negotiated procurement” scheme that would be farcical if it weren’t so ruinous. A May 24, 2018 report by Karol Ilagan and Malou Mangahas of the Philippine Center for Investigative Journalism (PCIJ) noted that Eddmari had also apparently secured contracts to build transitional shelters in Marawi. The PCIJ’s analysis of PhilGEPS data showed that in 2017 alone, Eddmari ranked 9th among 325 NHA contractors, cornering at least P962 million worth of projects from just three contracts. PCIJ cited a November 16, 2017 report by the state-run Philippine Information Agency (PIA), which listed Eddmari as one of the firms building transitional houses in Barangay Sagonsongan in Marawi. Yet, based on that 2018 PCIJ report, no notices of award or bidding documents could be found on the “transparency” websites of the NHA, DPWH, PhilGEPS, or the local governments of Marawi City and Lanao del Sur. Fast forward to December 2024: the Bases Conversion and Development Authority (BCDA), under president and CEO Joshua Bingcang, awarded the same firm a P240.78-million contract for the construction of the Bangko Sentral ng Pilipinas Access Road in New Clark City within the Clark Freeport and Special Economic Zone. So it stands: a firm once blacklisted by the NHA reemerges, phoenix-like, in the government’s portfolio. It is an emblem of how impermeable, and how shamelessly durable, the system remains. Eddmari’s hometown ties are uncomfortably close to rulers of Pampanga’s 4th District. Its current congressional representative is Anna York Cristina Puyat Bondoc, whose family has controlled Pampanga’s 4th District with dynastic regularity since the late 1980s. The congresswoman’s father, Emigdio, held the post until his untimely death in 1997. Her brother, Juan Pablo, then assumed the seat until 2004, after which Anna herself took over until 2013. Juan Pablo returned from 2013 to 2022, even rising to House deputy majority leader during the Duterte administration, before Anna reclaimed the position in 2022. Anna now serves as vice chairperson of the House appropriations committee, a body that controls, among other things, the lifeblood of public works spending of the Marcos administration. Interestingly, the congresswoman’s husband, Jayson S. Sagum, is the mayor of San Luis, a municipality located in the district she represents. It so happens that Eddmari Construction, the firm that repeatedly wins projects in Pampanga and elsewhere, lists its office address in San Juan, San Luis. And it so happens, too, that Eddmari is run by one Edgardo A. Sagum. One is, of course, enjoined to avoid hasty conclusions. But one may be forgiven for asking questions, as one might when encountering a string of curious coincidences in any detective novel. Are we seriously expected to believe this is all mere coincidence? What emerges is a template for national dysfunction. Floods in Luzon. War in Marawi. “Development” projects scattered across the archipelago. The sequence never changes: catastrophe is declared, a favored contractor is summoned, contracts are padded, transparency evaporates, accountability vanishes, and the people remain no safer than before. We are told, without blushing, that these are infrastructure projects. Let us not pervert the language. Flood control that controls nothing but the flow of taxpayers’ money is not flood control. It is failure that has been built into the very system. Filipinos, not just the residents of Arayat, suffer not from heaven’s curse, but from a government that has domesticated disaster into a business model. In this country, ruin is more profitable – disaster is not a misfortune but an investment opportunity. Pastilan. – Rappler.com How does this make you feel? </t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>BCDA,Budget Watch,Central Luzon,Clark Freeport Zone,DPWH,flood,flood control,Marawi rehabilitation,National Housing Authority,Philippine infrastructure</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>OPPO Reno14 Series 5G now available nationwide</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>https://www.rappler.com/brandrap/oppo-reno-14-series-5g-release/</t>
+        </is>
+      </c>
+      <c r="D34" s="2" t="n">
+        <v>45891.34430555555</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SUMMARY This is AI generated summarization, which may have errors. For context, always refer to the full article. Editor’s note: This press release is sponsored by OPPO and was handled by BrandRap, the sales and marketing arm of Rappler. No member of the news and editorial team participated in the publishing of this piece. The OPPO Reno14 Series 5G is now officially available in the Philippines, bringing next-level AI-powered imaging and creator-ready performance to anyone who wants to capture, connect, and share more. Built with powerful AI features and a design that puts creators first, the OPPO Reno14 Series 5G is your all-in-one creative companion. Still deciding if this is your next content device? Here are five reasons why. Low-light is no longer a problem. The OPPO Reno14 Series 5G’s Ultra-Clear Low-Light Camera System, plus a 3-Flash Design, delivers bright, sharp, natural-looking images in difficult lighting. Expect clean portraits and crisp Livephoto captures without harsh glare. Skip complicated post-production. AI Editor 2.0 creates quick, polished cuts using scene recognition. AI Recompose helps you fix framing and balance in a few taps, so your focus stays on the story. Take the shot where most phones stop. Rated IP66, IP68, and IP69, the OPPO Reno14 Series 5G lets you record 4K videos underwater. Use Underwater Mode for stable, clear footage during freshwater trips and pool sessions. Sometimes the best moments happen from a distance. The OPPO Reno14 Pro 5G features a 50MP telephoto lens with a dedicated flash that lets you zoom in closer without sacrificing detail, even in low light. From concerts to cityscapes, every capture is sharp and vibrant. Your #MainZoomMoment every time. From creators building their next reel to everyday users saving life’s milestones, the OPPO Reno14 Series 5G unlocks new possibilities with smooth performance, durable design, and creator-focused AI. It’s a phone that keeps up with your lifestyle and elevates your storytelling. Find the OPPO Reno14 Series 5G in all authorized OPPO Brand Stores and official OPPO online stores in Shopee , Lazada , and TikTok Shop . Redeem a limited-edition Make Your Moment carry-on and sticker set at select OPPO stores while supplies last. This is your moment. Capture it without limits with the OPPO Reno14 Series 5G. Visit www.oppo.com/ph/ or follow OPPO Philippines on Facebook , YouTube , and TikTok . – Rappler.com How does this make you feel? </t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>consumer electronics,electronics and gadgets,Oppo</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Negros Island’s first public cancer care hub opens in Bacolod</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>https://www.rappler.com/philippines/visayas/negros-island-region-first-public-cancer-care-hub-opens-bacolod-city/</t>
+        </is>
+      </c>
+      <c r="D35" s="2" t="n">
+        <v>45891.34392361111</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SUMMARY This is AI generated summarization, which may have errors. For context, always refer to the full article. CANCER CARE HUB. The Cancer Care Center is inaugurated in Bacolod City. It is the first government-run cancer hub in the Negros Island Region. Ambo Delilan/Rappler NEGROS OCCIDENTAL, Philippines – A government-run cancer care center in Bacolod City has opened its doors, offering what doctors and patients say is a lifeline for thousands battling the disease in the Negros Island Region (NIR). The Corazon Locsin Montelibano Memorial Regional Hospital (CLMMRH) inaugurated its P35 million Cancer Care Center (CCC) on Wednesday, August 20, the first public facility of its kind in the Negros Island Region (NIR). For patients like Nena (not her real name), a 48-year-old government employee battling Stage 2 breast cancer, the center brings hope closer to home. “I know this is no easy journey. Money is one among the challenges, but I have no choice. I have to face this reality, but I am determined as well to ace the battle,” she said. “Cancer, as I was told, is treatable. Thus, this CCC is a boon for us, more so with the poor or jobless ones, who are also having a silent battle against ‘Big C’ like us.” Dubbed the “Home of Hope,” the two-story facility can accommodate up to 40 cancer patients daily and is equipped for intravenous chemotherapy, biopsies, lumbar punctures, intrathecal chemotherapy and child life services. “This is much, much better compared to the usual six beds within the main hospital since we started offering chemotherapy in 2022,” said Dr. Norman Cabaya, an oncologist and focal person for the CCC. Radiotherapy is not yet available, but Cabaya said patients are referred free of charge to the Riverside Medical Center under a partnership agreement. Cabaya said they were waiting for funding approval from the Department of Health for radiotherapy service at CCC. “But, for sure, it will be soon,” he said. Dr. Joan Cerrada, CLMMRH chief, said the center aims to provide affordable treatment accessible through the Cancer Assistance Fund, PhilHealth’s Z-Benefit packages, and the Cancer and Supportive-Palliative Medicines Access Program (CSPMAP). Since March, 500 cancer patients have received support under CSPMAP, 1,000 through the Cancer Assistance Fund with up to P150,000 each, and 100 under the Z-Benefit packages. PhilHealth’s Z-Benefit packages cover breast cancer (up to P1.4 million), cervical cancer (P120,000), colon cancer (P150,000 to P300,000), rectal cancer (P150,000 to P400,000), prostate cancer (P100,000), and acute lymphocytic and lymphoblastic leukemia (up to P500,000), according to PhilHealth-Bacolod head Edgar Yocariza. Lung cancer, however, is not yet included despite being among the most prevalent types. Cancer is the second leading cause of death in the country after heart disease, according to the DOH. The Philippine Statistics Authority (PSA) reported 69,909 cancer deaths nationwide in 2023 and 42,870 from January to September 2024. Bacolod Mayor Greg Gasataya said the facility would serve the Negros Island Region, and not just residents of the city. Health officials said the CCC is designed to expand access to treatment in Negros Occidental, Negros Oriental, and Siquijor. “CLMMRH, as our regional apex hospital, must not only treat patients within its walls; it must also cultivate a network that ensures no cancer patient is left behind,” said DOH-NIR Director Razel Nikka Hao. – Rappler.com How does this make you feel? </t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>cancer,Department of Health,diseases and ailments,hospitals in the Philippines,Negros Island Region,public health</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Binay father and son acquitted in Makati car park building cases</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>https://www.rappler.com/philippines/metro-manila/jejomar-binay-father-son-acquitted-makati-car-park-building-cases/</t>
+        </is>
+      </c>
+      <c r="D36" s="2" t="n">
+        <v>45891.33361111111</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SUMMARY This is AI generated summarization, which may have errors. For context, always refer to the full article. MAYORS BOTH. Then-Makati mayor Junjun Binay greets his father, then-vice president Jejomar Binay, after the latter files his certificate of candidacy for president on October 12, 2015. Rappler MANILA, Philippines – The anti-graft court Sandiganbayan has cleared former vice president Jejomar Binay and his son Jejomar Jr. (Junjun), both ex-mayors of Makati City, of graft, falsification of public documents, and malversation of public funds over the allegedly overpriced car park building at city hall. Also acquitted on Friday, August 22, were the Binays’ co-accused, including 20 city government officials and two private contractors: Efren Canlas of Hilmarc’s Construction Company and Orlando Mateo of Mana Architecture and Interior Design. The Sandiganbayan said their guilt were not proven beyond reasonable doubt. The car park building, worth P2.2 billion, consisted of five phases. The first three were implemented when Jejomar Sr. was mayor, and the last two when Junjun succeeded his father, who had since been elected vice president in 2010. In 2015, a year before the presidential poll, a prolonged Senate investigation into the project was widely believed to have dragged down Jejomar Sr.’s earlier lead in pre-election surveys for president. – Rappler.com How does this make you feel? </t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Corruption in the Philippines,Jejomar Binay,LGUs in the Philippines,National Capital Region,Sandiganbayan</t>
         </is>
       </c>
     </row>

</xml_diff>